<commit_message>
added missing "path" attribute and checkmarks for submenus
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8E36F3-6F18-2F48-A992-F7E19041E5D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BACF29F-EFAC-AB46-ABA3-D70EC326951F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2380,9 +2380,6 @@
     <t>Visibility</t>
   </si>
   <si>
-    <t>File</t>
-  </si>
-  <si>
     <t>Script In</t>
   </si>
   <si>
@@ -3146,6 +3143,9 @@
   </si>
   <si>
     <t>Comment (Tooltip)</t>
+  </si>
+  <si>
+    <t>Path</t>
   </si>
 </sst>
 </file>
@@ -4029,9 +4029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W1" sqref="W1:Z1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4050,37 +4050,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>791</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>792</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>793</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>785</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -4094,7 +4094,7 @@
         <v>349</v>
       </c>
       <c r="D2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E2" t="s">
         <v>349</v>
@@ -4106,7 +4106,7 @@
         <v>543</v>
       </c>
       <c r="J2" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -4132,7 +4132,7 @@
         <v>350</v>
       </c>
       <c r="J3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -4146,7 +4146,7 @@
         <v>745</v>
       </c>
       <c r="D4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E4" t="s">
         <v>745</v>
@@ -4158,7 +4158,7 @@
         <v>746</v>
       </c>
       <c r="J4" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -4209,7 +4209,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -4224,7 +4224,7 @@
         <v>564</v>
       </c>
       <c r="J7" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -4235,7 +4235,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -4247,7 +4247,7 @@
         <v>560</v>
       </c>
       <c r="J8" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4258,10 +4258,10 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D9" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
@@ -4270,7 +4270,7 @@
         <v>562</v>
       </c>
       <c r="J9" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -4281,7 +4281,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D10" t="s">
         <v>259</v>
@@ -4296,7 +4296,7 @@
         <v>558</v>
       </c>
       <c r="J10" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -4307,13 +4307,13 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D11" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E11" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
@@ -4322,7 +4322,7 @@
         <v>566</v>
       </c>
       <c r="J11" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -4345,7 +4345,7 @@
         <v>554</v>
       </c>
       <c r="J12" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -4365,7 +4365,7 @@
         <v>550</v>
       </c>
       <c r="J13" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -4376,7 +4376,7 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F14" t="s">
         <v>3</v>
@@ -4385,7 +4385,7 @@
         <v>552</v>
       </c>
       <c r="J14" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -4408,7 +4408,7 @@
         <v>548</v>
       </c>
       <c r="J15" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -4419,7 +4419,7 @@
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
@@ -4431,7 +4431,7 @@
         <v>556</v>
       </c>
       <c r="J16" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -4471,7 +4471,7 @@
         <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -4491,7 +4491,7 @@
         <v>33</v>
       </c>
       <c r="J19" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -4511,7 +4511,7 @@
         <v>36</v>
       </c>
       <c r="J20" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -4531,7 +4531,7 @@
         <v>39</v>
       </c>
       <c r="J21" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -4568,7 +4568,7 @@
         <v>45</v>
       </c>
       <c r="J23" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -4588,7 +4588,7 @@
         <v>47</v>
       </c>
       <c r="J24" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -4608,7 +4608,7 @@
         <v>50</v>
       </c>
       <c r="J25" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -4628,7 +4628,7 @@
         <v>53</v>
       </c>
       <c r="J26" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -4648,7 +4648,7 @@
         <v>56</v>
       </c>
       <c r="J27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -4668,7 +4668,7 @@
         <v>59</v>
       </c>
       <c r="J28" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -4688,7 +4688,7 @@
         <v>62</v>
       </c>
       <c r="J29" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -4711,7 +4711,7 @@
         <v>627</v>
       </c>
       <c r="J30" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -4731,7 +4731,7 @@
         <v>623</v>
       </c>
       <c r="J31" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -4754,10 +4754,10 @@
         <v>634</v>
       </c>
       <c r="J32" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="K32" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -4768,7 +4768,7 @@
         <v>620</v>
       </c>
       <c r="D33" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F33" t="s">
         <v>3</v>
@@ -4777,7 +4777,7 @@
         <v>625</v>
       </c>
       <c r="J33" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -4800,7 +4800,7 @@
         <v>621</v>
       </c>
       <c r="J34" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -4811,7 +4811,7 @@
         <v>620</v>
       </c>
       <c r="D35" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E35" t="s">
         <v>620</v>
@@ -4823,7 +4823,7 @@
         <v>629</v>
       </c>
       <c r="J35" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -4843,7 +4843,7 @@
         <v>632</v>
       </c>
       <c r="J36" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -4851,13 +4851,13 @@
         <v>461</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D37" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F37" t="s">
         <v>3</v>
@@ -4866,7 +4866,7 @@
         <v>462</v>
       </c>
       <c r="J37" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -4892,7 +4892,7 @@
         <v>441</v>
       </c>
       <c r="J38" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -4918,7 +4918,7 @@
         <v>444</v>
       </c>
       <c r="J39" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -4944,7 +4944,7 @@
         <v>447</v>
       </c>
       <c r="J40" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -5085,7 +5085,7 @@
         <v>292</v>
       </c>
       <c r="J46" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -5111,7 +5111,7 @@
         <v>321</v>
       </c>
       <c r="J47" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -5137,7 +5137,7 @@
         <v>618</v>
       </c>
       <c r="J48" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -5154,7 +5154,7 @@
         <v>168</v>
       </c>
       <c r="E49" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F49" t="s">
         <v>3</v>
@@ -5163,10 +5163,10 @@
         <v>684</v>
       </c>
       <c r="J49" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="K49" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -5189,7 +5189,7 @@
         <v>682</v>
       </c>
       <c r="J50" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -5215,7 +5215,7 @@
         <v>355</v>
       </c>
       <c r="J51" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -5241,7 +5241,7 @@
         <v>358</v>
       </c>
       <c r="J52" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -5267,7 +5267,7 @@
         <v>423</v>
       </c>
       <c r="J53" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -5293,7 +5293,7 @@
         <v>426</v>
       </c>
       <c r="J54" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -5319,7 +5319,7 @@
         <v>429</v>
       </c>
       <c r="J55" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -5348,7 +5348,7 @@
         <v>755</v>
       </c>
       <c r="J56" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -5388,7 +5388,7 @@
         <v>75</v>
       </c>
       <c r="J58" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -5408,7 +5408,7 @@
         <v>77</v>
       </c>
       <c r="J59" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -5428,7 +5428,7 @@
         <v>79</v>
       </c>
       <c r="J60" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -5448,7 +5448,7 @@
         <v>81</v>
       </c>
       <c r="J61" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -5468,7 +5468,7 @@
         <v>42</v>
       </c>
       <c r="J62" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -5505,7 +5505,7 @@
         <v>86</v>
       </c>
       <c r="J64" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -5525,7 +5525,7 @@
         <v>88</v>
       </c>
       <c r="J65" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -5545,7 +5545,7 @@
         <v>90</v>
       </c>
       <c r="J66" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -5565,7 +5565,7 @@
         <v>92</v>
       </c>
       <c r="J67" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -5585,7 +5585,7 @@
         <v>94</v>
       </c>
       <c r="J68" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -5605,7 +5605,7 @@
         <v>96</v>
       </c>
       <c r="J69" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -5628,7 +5628,7 @@
         <v>318</v>
       </c>
       <c r="J70" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -5654,7 +5654,7 @@
         <v>438</v>
       </c>
       <c r="J71" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -5677,7 +5677,7 @@
         <v>434</v>
       </c>
       <c r="J72" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -5691,7 +5691,7 @@
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F73" t="s">
         <v>3</v>
@@ -5700,7 +5700,7 @@
         <v>436</v>
       </c>
       <c r="J73" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -5714,7 +5714,7 @@
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E74" t="s">
         <v>1</v>
@@ -5729,7 +5729,7 @@
         <v>432</v>
       </c>
       <c r="J74" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -5786,7 +5786,7 @@
         <v>16</v>
       </c>
       <c r="E77" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F77" t="s">
         <v>3</v>
@@ -5823,7 +5823,7 @@
         <v>114</v>
       </c>
       <c r="C79" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D79" t="s">
         <v>16</v>
@@ -5861,7 +5861,7 @@
         <v>491</v>
       </c>
       <c r="J80" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -5887,7 +5887,7 @@
         <v>493</v>
       </c>
       <c r="J81" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -5913,7 +5913,7 @@
         <v>495</v>
       </c>
       <c r="J82" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
@@ -5976,7 +5976,7 @@
         <v>122</v>
       </c>
       <c r="J85" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -5996,7 +5996,7 @@
         <v>124</v>
       </c>
       <c r="J86" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
@@ -6016,7 +6016,7 @@
         <v>126</v>
       </c>
       <c r="J87" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
@@ -6036,7 +6036,7 @@
         <v>128</v>
       </c>
       <c r="J88" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
@@ -6073,7 +6073,7 @@
         <v>131</v>
       </c>
       <c r="J90" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
@@ -6093,7 +6093,7 @@
         <v>133</v>
       </c>
       <c r="J91" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -6113,7 +6113,7 @@
         <v>135</v>
       </c>
       <c r="J92" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
@@ -6133,7 +6133,7 @@
         <v>137</v>
       </c>
       <c r="J93" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
@@ -6153,7 +6153,7 @@
         <v>139</v>
       </c>
       <c r="J94" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
@@ -6173,7 +6173,7 @@
         <v>141</v>
       </c>
       <c r="J95" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -6193,7 +6193,7 @@
         <v>143</v>
       </c>
       <c r="J96" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -6213,7 +6213,7 @@
         <v>145</v>
       </c>
       <c r="J97" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -6233,7 +6233,7 @@
         <v>147</v>
       </c>
       <c r="J98" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
@@ -6253,7 +6253,7 @@
         <v>149</v>
       </c>
       <c r="J99" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
@@ -6273,7 +6273,7 @@
         <v>151</v>
       </c>
       <c r="J100" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -6310,7 +6310,7 @@
         <v>154</v>
       </c>
       <c r="J102" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
@@ -6330,7 +6330,7 @@
         <v>156</v>
       </c>
       <c r="J103" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
@@ -6350,7 +6350,7 @@
         <v>158</v>
       </c>
       <c r="J104" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
@@ -6370,7 +6370,7 @@
         <v>160</v>
       </c>
       <c r="J105" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
@@ -6390,7 +6390,7 @@
         <v>162</v>
       </c>
       <c r="J106" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -6410,7 +6410,7 @@
         <v>164</v>
       </c>
       <c r="J107" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
@@ -6430,7 +6430,7 @@
         <v>166</v>
       </c>
       <c r="J108" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -6453,7 +6453,7 @@
         <v>170</v>
       </c>
       <c r="J109" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -6464,13 +6464,13 @@
         <v>168</v>
       </c>
       <c r="C110" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D110" t="s">
         <v>168</v>
       </c>
       <c r="E110" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F110" t="s">
         <v>6</v>
@@ -6482,7 +6482,7 @@
         <v>361</v>
       </c>
       <c r="J110" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -6519,7 +6519,7 @@
         <v>42</v>
       </c>
       <c r="J112" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
@@ -6530,7 +6530,7 @@
         <v>176</v>
       </c>
       <c r="C113" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D113" t="s">
         <v>16</v>
@@ -6542,7 +6542,7 @@
         <v>209</v>
       </c>
       <c r="J113" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
@@ -6582,7 +6582,7 @@
         <v>177</v>
       </c>
       <c r="J115" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
@@ -6665,7 +6665,7 @@
         <v>191</v>
       </c>
       <c r="J119" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
@@ -6877,7 +6877,7 @@
         <v>480</v>
       </c>
       <c r="B132" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C132" t="s">
         <v>464</v>
@@ -6892,7 +6892,7 @@
         <v>481</v>
       </c>
       <c r="J132" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
@@ -6900,7 +6900,7 @@
         <v>478</v>
       </c>
       <c r="B133" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C133" t="s">
         <v>464</v>
@@ -6915,7 +6915,7 @@
         <v>479</v>
       </c>
       <c r="J133" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
@@ -6923,7 +6923,7 @@
         <v>654</v>
       </c>
       <c r="B134" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C134" t="s">
         <v>642</v>
@@ -6938,7 +6938,7 @@
         <v>655</v>
       </c>
       <c r="J134" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
@@ -6946,7 +6946,7 @@
         <v>679</v>
       </c>
       <c r="B135" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C135" t="s">
         <v>667</v>
@@ -6961,7 +6961,7 @@
         <v>680</v>
       </c>
       <c r="J135" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
@@ -6969,7 +6969,7 @@
         <v>723</v>
       </c>
       <c r="B136" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C136" t="s">
         <v>711</v>
@@ -6984,7 +6984,7 @@
         <v>724</v>
       </c>
       <c r="J136" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
@@ -6992,10 +6992,10 @@
         <v>534</v>
       </c>
       <c r="B137" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C137" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D137" t="s">
         <v>259</v>
@@ -7010,7 +7010,7 @@
         <v>535</v>
       </c>
       <c r="J137" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
@@ -7018,16 +7018,16 @@
         <v>540</v>
       </c>
       <c r="B138" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C138" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>168</v>
       </c>
       <c r="E138" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F138" t="s">
         <v>3</v>
@@ -7036,7 +7036,7 @@
         <v>541</v>
       </c>
       <c r="J138" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
@@ -7044,16 +7044,16 @@
         <v>536</v>
       </c>
       <c r="B139" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C139" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D139" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E139" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F139" t="s">
         <v>3</v>
@@ -7062,7 +7062,7 @@
         <v>537</v>
       </c>
       <c r="J139" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
@@ -7070,10 +7070,10 @@
         <v>538</v>
       </c>
       <c r="B140" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C140" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D140" t="s">
         <v>186</v>
@@ -7085,7 +7085,7 @@
         <v>539</v>
       </c>
       <c r="J140" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
@@ -7093,13 +7093,13 @@
         <v>192</v>
       </c>
       <c r="B141" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D141" t="s">
         <v>16</v>
       </c>
       <c r="E141" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F141" t="s">
         <v>6</v>
@@ -7128,7 +7128,7 @@
         <v>211</v>
       </c>
       <c r="J142" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
@@ -7148,7 +7148,7 @@
         <v>213</v>
       </c>
       <c r="J143" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -7168,7 +7168,7 @@
         <v>215</v>
       </c>
       <c r="J144" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -7188,7 +7188,7 @@
         <v>217</v>
       </c>
       <c r="J145" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
@@ -7208,7 +7208,7 @@
         <v>219</v>
       </c>
       <c r="J146" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
@@ -7245,7 +7245,7 @@
         <v>222</v>
       </c>
       <c r="J148" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
@@ -7265,7 +7265,7 @@
         <v>224</v>
       </c>
       <c r="J149" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
@@ -7285,7 +7285,7 @@
         <v>226</v>
       </c>
       <c r="J150" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
@@ -7305,7 +7305,7 @@
         <v>228</v>
       </c>
       <c r="J151" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
@@ -7325,7 +7325,7 @@
         <v>230</v>
       </c>
       <c r="J152" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
@@ -7345,7 +7345,7 @@
         <v>232</v>
       </c>
       <c r="J153" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
@@ -7415,7 +7415,7 @@
         <v>594</v>
       </c>
       <c r="J156" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
@@ -7435,7 +7435,7 @@
         <v>590</v>
       </c>
       <c r="J157" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
@@ -7446,7 +7446,7 @@
         <v>236</v>
       </c>
       <c r="D158" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F158" t="s">
         <v>3</v>
@@ -7455,7 +7455,7 @@
         <v>592</v>
       </c>
       <c r="J158" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
@@ -7478,7 +7478,7 @@
         <v>588</v>
       </c>
       <c r="J159" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
@@ -7489,7 +7489,7 @@
         <v>236</v>
       </c>
       <c r="D160" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E160" t="s">
         <v>236</v>
@@ -7501,7 +7501,7 @@
         <v>596</v>
       </c>
       <c r="J160" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
@@ -7524,7 +7524,7 @@
         <v>604</v>
       </c>
       <c r="J161" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
@@ -7544,7 +7544,7 @@
         <v>600</v>
       </c>
       <c r="J162" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
@@ -7555,7 +7555,7 @@
         <v>239</v>
       </c>
       <c r="D163" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F163" t="s">
         <v>3</v>
@@ -7564,7 +7564,7 @@
         <v>602</v>
       </c>
       <c r="J163" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
@@ -7587,7 +7587,7 @@
         <v>598</v>
       </c>
       <c r="J164" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
@@ -7598,7 +7598,7 @@
         <v>239</v>
       </c>
       <c r="D165" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E165" t="s">
         <v>239</v>
@@ -7610,7 +7610,7 @@
         <v>606</v>
       </c>
       <c r="J165" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
@@ -7621,13 +7621,13 @@
         <v>16</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F166" t="s">
         <v>6</v>
@@ -7647,13 +7647,13 @@
         <v>16</v>
       </c>
       <c r="C167" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E167" s="2" t="s">
         <v>826</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>827</v>
       </c>
       <c r="F167" t="s">
         <v>6</v>
@@ -7688,7 +7688,7 @@
         <v>460</v>
       </c>
       <c r="J168" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
@@ -7711,7 +7711,7 @@
         <v>454</v>
       </c>
       <c r="J169" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
@@ -7725,7 +7725,7 @@
         <v>451</v>
       </c>
       <c r="D170" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F170" t="s">
         <v>3</v>
@@ -7734,7 +7734,7 @@
         <v>458</v>
       </c>
       <c r="J170" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.2">
@@ -7760,7 +7760,7 @@
         <v>452</v>
       </c>
       <c r="J171" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.2">
@@ -7774,7 +7774,7 @@
         <v>451</v>
       </c>
       <c r="D172" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E172" t="s">
         <v>451</v>
@@ -7786,7 +7786,7 @@
         <v>456</v>
       </c>
       <c r="J172" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
@@ -7812,7 +7812,7 @@
         <v>473</v>
       </c>
       <c r="J173" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
@@ -7835,7 +7835,7 @@
         <v>467</v>
       </c>
       <c r="J174" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.2">
@@ -7849,7 +7849,7 @@
         <v>464</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F175" t="s">
         <v>3</v>
@@ -7858,7 +7858,7 @@
         <v>469</v>
       </c>
       <c r="J175" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
@@ -7884,7 +7884,7 @@
         <v>465</v>
       </c>
       <c r="J176" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.2">
@@ -7907,7 +7907,7 @@
         <v>477</v>
       </c>
       <c r="J177" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.2">
@@ -7921,7 +7921,7 @@
         <v>464</v>
       </c>
       <c r="D178" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F178" t="s">
         <v>3</v>
@@ -7930,7 +7930,7 @@
         <v>471</v>
       </c>
       <c r="J178" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.2">
@@ -7953,7 +7953,7 @@
         <v>475</v>
       </c>
       <c r="J179" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
@@ -7979,7 +7979,7 @@
         <v>637</v>
       </c>
       <c r="J180" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.2">
@@ -8005,7 +8005,7 @@
         <v>506</v>
       </c>
       <c r="J181" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
@@ -8028,7 +8028,7 @@
         <v>500</v>
       </c>
       <c r="J182" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
@@ -8042,7 +8042,7 @@
         <v>497</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F183" t="s">
         <v>3</v>
@@ -8051,7 +8051,7 @@
         <v>502</v>
       </c>
       <c r="J183" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
@@ -8077,7 +8077,7 @@
         <v>498</v>
       </c>
       <c r="J184" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
@@ -8091,7 +8091,7 @@
         <v>497</v>
       </c>
       <c r="D185" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E185" t="s">
         <v>497</v>
@@ -8103,7 +8103,7 @@
         <v>504</v>
       </c>
       <c r="J185" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
@@ -8126,7 +8126,7 @@
         <v>487</v>
       </c>
       <c r="J186" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
@@ -8143,7 +8143,7 @@
         <v>16</v>
       </c>
       <c r="E187" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="F187" t="s">
         <v>3</v>
@@ -8152,7 +8152,7 @@
         <v>546</v>
       </c>
       <c r="J187" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
@@ -8178,7 +8178,7 @@
         <v>575</v>
       </c>
       <c r="J188" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
@@ -8201,7 +8201,7 @@
         <v>571</v>
       </c>
       <c r="J189" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
@@ -8215,7 +8215,7 @@
         <v>568</v>
       </c>
       <c r="D190" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F190" t="s">
         <v>3</v>
@@ -8224,7 +8224,7 @@
         <v>573</v>
       </c>
       <c r="J190" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
@@ -8250,7 +8250,7 @@
         <v>569</v>
       </c>
       <c r="J191" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.2">
@@ -8264,7 +8264,7 @@
         <v>568</v>
       </c>
       <c r="D192" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E192" t="s">
         <v>568</v>
@@ -8276,7 +8276,7 @@
         <v>577</v>
       </c>
       <c r="J192" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="193" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -8302,7 +8302,7 @@
         <v>580</v>
       </c>
       <c r="J193" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.2">
@@ -8325,7 +8325,7 @@
         <v>582</v>
       </c>
       <c r="J194" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.2">
@@ -8336,7 +8336,7 @@
         <v>16</v>
       </c>
       <c r="C195" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D195" t="s">
         <v>13</v>
@@ -8351,7 +8351,7 @@
         <v>734</v>
       </c>
       <c r="J195" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.2">
@@ -8362,7 +8362,7 @@
         <v>16</v>
       </c>
       <c r="C196" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D196" t="s">
         <v>13</v>
@@ -8374,7 +8374,7 @@
         <v>730</v>
       </c>
       <c r="J196" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.2">
@@ -8385,10 +8385,10 @@
         <v>16</v>
       </c>
       <c r="C197" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D197" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F197" t="s">
         <v>3</v>
@@ -8397,7 +8397,7 @@
         <v>732</v>
       </c>
       <c r="J197" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.2">
@@ -8408,7 +8408,7 @@
         <v>16</v>
       </c>
       <c r="C198" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D198" t="s">
         <v>259</v>
@@ -8423,7 +8423,7 @@
         <v>728</v>
       </c>
       <c r="J198" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.2">
@@ -8434,10 +8434,10 @@
         <v>16</v>
       </c>
       <c r="C199" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D199" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F199" t="s">
         <v>3</v>
@@ -8446,7 +8446,7 @@
         <v>736</v>
       </c>
       <c r="J199" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.2">
@@ -8472,7 +8472,7 @@
         <v>611</v>
       </c>
       <c r="J200" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.2">
@@ -8498,7 +8498,7 @@
         <v>613</v>
       </c>
       <c r="J201" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.2">
@@ -8524,7 +8524,7 @@
         <v>615</v>
       </c>
       <c r="J202" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.2">
@@ -8535,10 +8535,10 @@
         <v>16</v>
       </c>
       <c r="C203" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D203" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F203" t="s">
         <v>3</v>
@@ -8547,7 +8547,7 @@
         <v>489</v>
       </c>
       <c r="J203" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.2">
@@ -8561,7 +8561,7 @@
         <v>639</v>
       </c>
       <c r="D204" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E204" t="s">
         <v>639</v>
@@ -8573,7 +8573,7 @@
         <v>640</v>
       </c>
       <c r="J204" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.2">
@@ -8599,10 +8599,10 @@
         <v>773</v>
       </c>
       <c r="J205" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="K205" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.2">
@@ -8619,13 +8619,13 @@
         <v>16</v>
       </c>
       <c r="E206" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F206" t="s">
         <v>6</v>
       </c>
       <c r="J206" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.2">
@@ -8651,7 +8651,7 @@
         <v>649</v>
       </c>
       <c r="J207" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.2">
@@ -8674,7 +8674,7 @@
         <v>645</v>
       </c>
       <c r="J208" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.2">
@@ -8688,7 +8688,7 @@
         <v>642</v>
       </c>
       <c r="D209" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F209" t="s">
         <v>3</v>
@@ -8697,7 +8697,7 @@
         <v>647</v>
       </c>
       <c r="J209" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.2">
@@ -8723,7 +8723,7 @@
         <v>643</v>
       </c>
       <c r="J210" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.2">
@@ -8737,7 +8737,7 @@
         <v>642</v>
       </c>
       <c r="D211" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E211" t="s">
         <v>642</v>
@@ -8749,7 +8749,7 @@
         <v>653</v>
       </c>
       <c r="J211" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.2">
@@ -8772,7 +8772,7 @@
         <v>651</v>
       </c>
       <c r="J212" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.2">
@@ -8798,7 +8798,7 @@
         <v>674</v>
       </c>
       <c r="J213" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.2">
@@ -8821,7 +8821,7 @@
         <v>670</v>
       </c>
       <c r="J214" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.2">
@@ -8835,7 +8835,7 @@
         <v>667</v>
       </c>
       <c r="D215" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F215" t="s">
         <v>3</v>
@@ -8844,7 +8844,7 @@
         <v>672</v>
       </c>
       <c r="J215" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.2">
@@ -8870,7 +8870,7 @@
         <v>668</v>
       </c>
       <c r="J216" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.2">
@@ -8884,7 +8884,7 @@
         <v>667</v>
       </c>
       <c r="D217" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E217" t="s">
         <v>667</v>
@@ -8896,7 +8896,7 @@
         <v>678</v>
       </c>
       <c r="J217" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.2">
@@ -8919,7 +8919,7 @@
         <v>676</v>
       </c>
       <c r="J218" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.2">
@@ -8930,7 +8930,7 @@
         <v>16</v>
       </c>
       <c r="C219" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D219" t="s">
         <v>71</v>
@@ -8945,10 +8945,10 @@
         <v>586</v>
       </c>
       <c r="J219" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="K219" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.2">
@@ -8959,7 +8959,7 @@
         <v>16</v>
       </c>
       <c r="C220" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D220" t="s">
         <v>176</v>
@@ -8971,10 +8971,10 @@
         <v>584</v>
       </c>
       <c r="J220" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="K220" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.2">
@@ -8985,7 +8985,7 @@
         <v>16</v>
       </c>
       <c r="C221" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D221" t="s">
         <v>13</v>
@@ -9000,7 +9000,7 @@
         <v>663</v>
       </c>
       <c r="J221" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.2">
@@ -9011,7 +9011,7 @@
         <v>16</v>
       </c>
       <c r="C222" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D222" t="s">
         <v>13</v>
@@ -9023,7 +9023,7 @@
         <v>659</v>
       </c>
       <c r="J222" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.2">
@@ -9034,10 +9034,10 @@
         <v>16</v>
       </c>
       <c r="C223" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D223" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F223" t="s">
         <v>3</v>
@@ -9046,7 +9046,7 @@
         <v>661</v>
       </c>
       <c r="J223" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.2">
@@ -9057,7 +9057,7 @@
         <v>16</v>
       </c>
       <c r="C224" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D224" t="s">
         <v>259</v>
@@ -9072,7 +9072,7 @@
         <v>657</v>
       </c>
       <c r="J224" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.2">
@@ -9083,13 +9083,13 @@
         <v>16</v>
       </c>
       <c r="C225" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D225" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E225" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F225" t="s">
         <v>3</v>
@@ -9098,7 +9098,7 @@
         <v>665</v>
       </c>
       <c r="J225" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.2">
@@ -9124,7 +9124,7 @@
         <v>686</v>
       </c>
       <c r="J226" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.2">
@@ -9150,7 +9150,7 @@
         <v>718</v>
       </c>
       <c r="J227" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.2">
@@ -9173,7 +9173,7 @@
         <v>714</v>
       </c>
       <c r="J228" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.2">
@@ -9187,7 +9187,7 @@
         <v>711</v>
       </c>
       <c r="D229" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F229" t="s">
         <v>3</v>
@@ -9196,7 +9196,7 @@
         <v>716</v>
       </c>
       <c r="J229" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.2">
@@ -9222,7 +9222,7 @@
         <v>712</v>
       </c>
       <c r="J230" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.2">
@@ -9236,7 +9236,7 @@
         <v>711</v>
       </c>
       <c r="D231" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E231" t="s">
         <v>711</v>
@@ -9248,7 +9248,7 @@
         <v>722</v>
       </c>
       <c r="J231" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
@@ -9271,7 +9271,7 @@
         <v>720</v>
       </c>
       <c r="J232" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -9297,7 +9297,7 @@
         <v>517</v>
       </c>
       <c r="J233" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.2">
@@ -9320,7 +9320,7 @@
         <v>511</v>
       </c>
       <c r="J234" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.2">
@@ -9334,7 +9334,7 @@
         <v>508</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F235" t="s">
         <v>3</v>
@@ -9343,7 +9343,7 @@
         <v>513</v>
       </c>
       <c r="J235" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
@@ -9369,7 +9369,7 @@
         <v>509</v>
       </c>
       <c r="J236" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
@@ -9386,7 +9386,7 @@
         <v>168</v>
       </c>
       <c r="E237" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F237" t="s">
         <v>3</v>
@@ -9395,7 +9395,7 @@
         <v>521</v>
       </c>
       <c r="J237" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
@@ -9409,7 +9409,7 @@
         <v>508</v>
       </c>
       <c r="D238" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E238" t="s">
         <v>508</v>
@@ -9421,7 +9421,7 @@
         <v>515</v>
       </c>
       <c r="J238" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
@@ -9444,7 +9444,7 @@
         <v>519</v>
       </c>
       <c r="J239" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.2">
@@ -9455,7 +9455,7 @@
         <v>16</v>
       </c>
       <c r="C240" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D240" t="s">
         <v>13</v>
@@ -9470,7 +9470,7 @@
         <v>529</v>
       </c>
       <c r="J240" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.2">
@@ -9481,7 +9481,7 @@
         <v>16</v>
       </c>
       <c r="C241" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D241" t="s">
         <v>13</v>
@@ -9493,7 +9493,7 @@
         <v>525</v>
       </c>
       <c r="J241" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.2">
@@ -9504,10 +9504,10 @@
         <v>16</v>
       </c>
       <c r="C242" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D242" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F242" t="s">
         <v>3</v>
@@ -9516,7 +9516,7 @@
         <v>527</v>
       </c>
       <c r="J242" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.2">
@@ -9527,7 +9527,7 @@
         <v>16</v>
       </c>
       <c r="C243" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D243" t="s">
         <v>259</v>
@@ -9542,7 +9542,7 @@
         <v>523</v>
       </c>
       <c r="J243" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.2">
@@ -9553,13 +9553,13 @@
         <v>16</v>
       </c>
       <c r="C244" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>168</v>
       </c>
       <c r="E244" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F244" t="s">
         <v>3</v>
@@ -9568,7 +9568,7 @@
         <v>533</v>
       </c>
       <c r="J244" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.2">
@@ -9579,7 +9579,7 @@
         <v>16</v>
       </c>
       <c r="C245" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D245" t="s">
         <v>186</v>
@@ -9591,7 +9591,7 @@
         <v>531</v>
       </c>
       <c r="J245" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.2">
@@ -9617,7 +9617,7 @@
         <v>739</v>
       </c>
       <c r="J246" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -9643,7 +9643,7 @@
         <v>741</v>
       </c>
       <c r="J247" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.2">
@@ -9669,7 +9669,7 @@
         <v>743</v>
       </c>
       <c r="J248" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.2">
@@ -9680,13 +9680,13 @@
         <v>16</v>
       </c>
       <c r="C249" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D249" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E249" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F249" t="s">
         <v>3</v>
@@ -9695,7 +9695,7 @@
         <v>757</v>
       </c>
       <c r="J249" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
@@ -9709,7 +9709,7 @@
         <v>483</v>
       </c>
       <c r="D250" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E250" t="s">
         <v>483</v>
@@ -9721,7 +9721,7 @@
         <v>484</v>
       </c>
       <c r="J250" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
@@ -9747,7 +9747,7 @@
         <v>766</v>
       </c>
       <c r="J251" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
@@ -9770,7 +9770,7 @@
         <v>762</v>
       </c>
       <c r="J252" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.2">
@@ -9784,7 +9784,7 @@
         <v>759</v>
       </c>
       <c r="D253" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F253" t="s">
         <v>3</v>
@@ -9793,7 +9793,7 @@
         <v>764</v>
       </c>
       <c r="J253" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.2">
@@ -9819,7 +9819,7 @@
         <v>760</v>
       </c>
       <c r="J254" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.2">
@@ -9833,7 +9833,7 @@
         <v>759</v>
       </c>
       <c r="D255" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E255" t="s">
         <v>759</v>
@@ -9845,7 +9845,7 @@
         <v>768</v>
       </c>
       <c r="J255" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.2">
@@ -9862,7 +9862,7 @@
         <v>16</v>
       </c>
       <c r="E256" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F256" t="s">
         <v>3</v>
@@ -9871,7 +9871,7 @@
         <v>771</v>
       </c>
       <c r="J256" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.2">
@@ -9897,7 +9897,7 @@
         <v>782</v>
       </c>
       <c r="J257" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.2">
@@ -9920,7 +9920,7 @@
         <v>778</v>
       </c>
       <c r="J258" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.2">
@@ -9934,7 +9934,7 @@
         <v>775</v>
       </c>
       <c r="D259" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F259" t="s">
         <v>3</v>
@@ -9943,7 +9943,7 @@
         <v>780</v>
       </c>
       <c r="J259" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.2">
@@ -9969,7 +9969,7 @@
         <v>776</v>
       </c>
       <c r="J260" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.2">
@@ -9983,7 +9983,7 @@
         <v>775</v>
       </c>
       <c r="D261" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E261" t="s">
         <v>775</v>
@@ -10049,7 +10049,7 @@
         <v>250</v>
       </c>
       <c r="J264" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.2">
@@ -10089,7 +10089,7 @@
         <v>257</v>
       </c>
       <c r="J266" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.2">
@@ -10129,7 +10129,7 @@
         <v>263</v>
       </c>
       <c r="J268" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.2">
@@ -10149,7 +10149,7 @@
         <v>265</v>
       </c>
       <c r="J269" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.2">
@@ -10163,7 +10163,7 @@
         <v>176</v>
       </c>
       <c r="E270" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F270" t="s">
         <v>6</v>
@@ -10183,7 +10183,7 @@
         <v>176</v>
       </c>
       <c r="E271" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F271" t="s">
         <v>3</v>
@@ -10192,7 +10192,7 @@
         <v>270</v>
       </c>
       <c r="J271" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.2">
@@ -10212,7 +10212,7 @@
         <v>267</v>
       </c>
       <c r="J272" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.2">
@@ -10232,7 +10232,7 @@
         <v>42</v>
       </c>
       <c r="J273" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.2">
@@ -10243,7 +10243,7 @@
         <v>16</v>
       </c>
       <c r="D274" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E274" t="s">
         <v>16</v>
@@ -10255,7 +10255,7 @@
         <v>608</v>
       </c>
       <c r="J274" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.2">
@@ -10275,7 +10275,7 @@
         <v>272</v>
       </c>
       <c r="J275" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.2">
@@ -10298,7 +10298,7 @@
         <v>275</v>
       </c>
       <c r="J276" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.2">
@@ -10318,7 +10318,7 @@
         <v>277</v>
       </c>
       <c r="J277" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.2">
@@ -10338,7 +10338,7 @@
         <v>282</v>
       </c>
       <c r="J278" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.2">
@@ -10352,7 +10352,7 @@
         <v>352</v>
       </c>
       <c r="E279" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F279" t="s">
         <v>6</v>
@@ -10364,7 +10364,7 @@
         <v>280</v>
       </c>
       <c r="J279" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.2">
@@ -10384,7 +10384,7 @@
         <v>284</v>
       </c>
       <c r="J280" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.2">
@@ -10404,7 +10404,7 @@
         <v>286</v>
       </c>
       <c r="J281" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.2">
@@ -10427,7 +10427,7 @@
         <v>415</v>
       </c>
       <c r="J282" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.2">
@@ -10447,7 +10447,7 @@
         <v>289</v>
       </c>
       <c r="J283" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.2">
@@ -10467,7 +10467,7 @@
         <v>294</v>
       </c>
       <c r="J284" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.2">
@@ -10487,7 +10487,7 @@
         <v>296</v>
       </c>
       <c r="J285" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.2">
@@ -10507,7 +10507,7 @@
         <v>298</v>
       </c>
       <c r="J286" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.2">
@@ -10527,7 +10527,7 @@
         <v>300</v>
       </c>
       <c r="J287" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.2">
@@ -10547,7 +10547,7 @@
         <v>302</v>
       </c>
       <c r="J288" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.2">
@@ -10567,7 +10567,7 @@
         <v>42</v>
       </c>
       <c r="J289" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.2">
@@ -10587,7 +10587,7 @@
         <v>305</v>
       </c>
       <c r="J290" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.2">
@@ -10607,7 +10607,7 @@
         <v>307</v>
       </c>
       <c r="J291" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.2">
@@ -10627,7 +10627,7 @@
         <v>309</v>
       </c>
       <c r="J292" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.2">
@@ -10647,7 +10647,7 @@
         <v>311</v>
       </c>
       <c r="J293" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.2">
@@ -10667,7 +10667,7 @@
         <v>313</v>
       </c>
       <c r="J294" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.2">
@@ -10687,7 +10687,7 @@
         <v>315</v>
       </c>
       <c r="J295" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
@@ -10695,7 +10695,7 @@
         <v>693</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D296" t="s">
         <v>13</v>
@@ -10710,7 +10710,7 @@
         <v>694</v>
       </c>
       <c r="J296" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
@@ -10718,7 +10718,7 @@
         <v>689</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D297" t="s">
         <v>13</v>
@@ -10730,7 +10730,7 @@
         <v>690</v>
       </c>
       <c r="J297" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
@@ -10738,10 +10738,10 @@
         <v>691</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D298" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F298" t="s">
         <v>3</v>
@@ -10750,7 +10750,7 @@
         <v>692</v>
       </c>
       <c r="J298" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.2">
@@ -10758,7 +10758,7 @@
         <v>687</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D299" t="s">
         <v>259</v>
@@ -10773,7 +10773,7 @@
         <v>688</v>
       </c>
       <c r="J299" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.2">
@@ -10781,13 +10781,13 @@
         <v>695</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D300" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E300" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F300" t="s">
         <v>3</v>
@@ -10796,7 +10796,7 @@
         <v>696</v>
       </c>
       <c r="J300" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
@@ -10816,7 +10816,7 @@
         <v>323</v>
       </c>
       <c r="J301" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.2">
@@ -10836,7 +10836,7 @@
         <v>325</v>
       </c>
       <c r="J302" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.2">
@@ -10856,7 +10856,7 @@
         <v>327</v>
       </c>
       <c r="J303" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.2">
@@ -10876,7 +10876,7 @@
         <v>329</v>
       </c>
       <c r="J304" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.2">
@@ -10896,7 +10896,7 @@
         <v>331</v>
       </c>
       <c r="J305" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.2">
@@ -10916,7 +10916,7 @@
         <v>42</v>
       </c>
       <c r="J306" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.2">
@@ -10936,7 +10936,7 @@
         <v>334</v>
       </c>
       <c r="J307" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.2">
@@ -10956,7 +10956,7 @@
         <v>336</v>
       </c>
       <c r="J308" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.2">
@@ -10976,7 +10976,7 @@
         <v>338</v>
       </c>
       <c r="J309" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.2">
@@ -10996,7 +10996,7 @@
         <v>340</v>
       </c>
       <c r="J310" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.2">
@@ -11016,7 +11016,7 @@
         <v>342</v>
       </c>
       <c r="J311" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.2">
@@ -11036,7 +11036,7 @@
         <v>344</v>
       </c>
       <c r="J312" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.2">
@@ -11059,7 +11059,7 @@
         <v>347</v>
       </c>
       <c r="J313" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.2">
@@ -11082,7 +11082,7 @@
         <v>705</v>
       </c>
       <c r="J314" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.2">
@@ -11102,7 +11102,7 @@
         <v>701</v>
       </c>
       <c r="J315" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.2">
@@ -11113,7 +11113,7 @@
         <v>698</v>
       </c>
       <c r="D316" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F316" t="s">
         <v>3</v>
@@ -11122,7 +11122,7 @@
         <v>703</v>
       </c>
       <c r="J316" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.2">
@@ -11145,7 +11145,7 @@
         <v>699</v>
       </c>
       <c r="J317" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.2">
@@ -11156,7 +11156,7 @@
         <v>698</v>
       </c>
       <c r="D318" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E318" t="s">
         <v>698</v>
@@ -11168,7 +11168,7 @@
         <v>707</v>
       </c>
       <c r="J318" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
@@ -11188,7 +11188,7 @@
         <v>709</v>
       </c>
       <c r="J319" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.2">
@@ -11211,7 +11211,7 @@
         <v>365</v>
       </c>
       <c r="J320" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.2">
@@ -11231,7 +11231,7 @@
         <v>367</v>
       </c>
       <c r="J321" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.2">
@@ -11251,7 +11251,7 @@
         <v>369</v>
       </c>
       <c r="J322" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.2">
@@ -11271,7 +11271,7 @@
         <v>371</v>
       </c>
       <c r="J323" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.2">
@@ -11291,7 +11291,7 @@
         <v>373</v>
       </c>
       <c r="J324" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.2">
@@ -11311,7 +11311,7 @@
         <v>375</v>
       </c>
       <c r="J325" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.2">
@@ -11331,7 +11331,7 @@
         <v>42</v>
       </c>
       <c r="J326" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.2">
@@ -11342,7 +11342,7 @@
         <v>55</v>
       </c>
       <c r="D327" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E327" t="s">
         <v>55</v>
@@ -11354,7 +11354,7 @@
         <v>726</v>
       </c>
       <c r="J327" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.2">
@@ -11374,7 +11374,7 @@
         <v>378</v>
       </c>
       <c r="J328" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="329" spans="1:10" x14ac:dyDescent="0.2">
@@ -11394,7 +11394,7 @@
         <v>380</v>
       </c>
       <c r="J329" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.2">
@@ -11414,7 +11414,7 @@
         <v>382</v>
       </c>
       <c r="J330" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.2">
@@ -11434,7 +11434,7 @@
         <v>384</v>
       </c>
       <c r="J331" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.2">
@@ -11454,7 +11454,7 @@
         <v>386</v>
       </c>
       <c r="J332" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.2">
@@ -11474,7 +11474,7 @@
         <v>388</v>
       </c>
       <c r="J333" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.2">
@@ -11494,7 +11494,7 @@
         <v>390</v>
       </c>
       <c r="J334" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.2">
@@ -11514,7 +11514,7 @@
         <v>392</v>
       </c>
       <c r="J335" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.2">
@@ -11534,7 +11534,7 @@
         <v>394</v>
       </c>
       <c r="J336" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.2">
@@ -11554,7 +11554,7 @@
         <v>396</v>
       </c>
       <c r="J337" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.2">
@@ -11574,7 +11574,7 @@
         <v>398</v>
       </c>
       <c r="J338" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.2">
@@ -11594,7 +11594,7 @@
         <v>42</v>
       </c>
       <c r="J339" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="340" spans="1:10" x14ac:dyDescent="0.2">
@@ -11614,7 +11614,7 @@
         <v>401</v>
       </c>
       <c r="J340" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.2">
@@ -11634,7 +11634,7 @@
         <v>403</v>
       </c>
       <c r="J341" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.2">
@@ -11654,7 +11654,7 @@
         <v>405</v>
       </c>
       <c r="J342" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
@@ -11674,7 +11674,7 @@
         <v>407</v>
       </c>
       <c r="J343" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.2">
@@ -11694,7 +11694,7 @@
         <v>409</v>
       </c>
       <c r="J344" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.2">
@@ -11714,7 +11714,7 @@
         <v>411</v>
       </c>
       <c r="J345" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.2">
@@ -11725,7 +11725,7 @@
         <v>288</v>
       </c>
       <c r="C346" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D346" t="s">
         <v>16</v>
@@ -11737,7 +11737,7 @@
         <v>42</v>
       </c>
       <c r="J346" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.2">
@@ -11748,13 +11748,13 @@
         <v>288</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D347" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E347" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F347" t="s">
         <v>3</v>
@@ -11763,7 +11763,7 @@
         <v>449</v>
       </c>
       <c r="J347" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.2">
@@ -11783,7 +11783,7 @@
         <v>417</v>
       </c>
       <c r="J348" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.2">
@@ -11797,7 +11797,7 @@
         <v>288</v>
       </c>
       <c r="E349" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F349" t="s">
         <v>6</v>
@@ -11806,7 +11806,7 @@
         <v>42</v>
       </c>
       <c r="J349" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.2">
@@ -11820,7 +11820,7 @@
         <v>288</v>
       </c>
       <c r="E350" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F350" t="s">
         <v>6</v>
@@ -11829,7 +11829,7 @@
         <v>42</v>
       </c>
       <c r="J350" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.2">
@@ -11852,7 +11852,7 @@
         <v>752</v>
       </c>
       <c r="J351" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.2">
@@ -11872,7 +11872,7 @@
         <v>748</v>
       </c>
       <c r="J352" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.2">
@@ -11883,7 +11883,7 @@
         <v>193</v>
       </c>
       <c r="D353" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F353" t="s">
         <v>3</v>
@@ -11892,7 +11892,7 @@
         <v>750</v>
       </c>
       <c r="J353" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixes for saving/read preferences, loading demo and setting menus correctly
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8FD245-B607-D742-B120-6566C59B0189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DD3CEB-9A6C-E043-B449-0AF7FD06F81C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38360" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3103" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3106" uniqueCount="1202">
   <si>
     <t>Amharic-Latin-BGN.xml</t>
   </si>
@@ -3247,9 +3247,6 @@
     <t>Ethi</t>
   </si>
   <si>
-    <t>Ethi_Latn</t>
-  </si>
-  <si>
     <t>ka</t>
   </si>
   <si>
@@ -3626,6 +3623,9 @@
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>Aethiopica_Latn</t>
   </si>
 </sst>
 </file>
@@ -4509,9 +4509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M355"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D352" sqref="A352:XFD354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4536,10 +4536,10 @@
         <v>1040</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1200</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1201</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>786</v>
@@ -4577,10 +4577,10 @@
         <v>542</v>
       </c>
       <c r="B2" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C2" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -4609,10 +4609,10 @@
         <v>348</v>
       </c>
       <c r="B3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C3" t="s">
         <v>1110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1111</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -4641,10 +4641,10 @@
         <v>744</v>
       </c>
       <c r="B4" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C4" t="s">
         <v>1188</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1189</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -4725,10 +4725,10 @@
         <v>563</v>
       </c>
       <c r="B7" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C7" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -4757,7 +4757,7 @@
         <v>559</v>
       </c>
       <c r="B8" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C8" t="s">
         <v>1050</v>
@@ -4786,10 +4786,10 @@
         <v>561</v>
       </c>
       <c r="B9" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C9" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -4815,7 +4815,7 @@
         <v>557</v>
       </c>
       <c r="B10" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C10" t="s">
         <v>1045</v>
@@ -4847,10 +4847,10 @@
         <v>565</v>
       </c>
       <c r="B11" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C11" t="s">
         <v>1154</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1155</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
@@ -4882,7 +4882,7 @@
         <v>1054</v>
       </c>
       <c r="C12" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -4937,7 +4937,7 @@
         <v>1054</v>
       </c>
       <c r="C14" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -4992,7 +4992,7 @@
         <v>1054</v>
       </c>
       <c r="C16" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -5353,10 +5353,10 @@
         <v>626</v>
       </c>
       <c r="B30" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C30" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D30" t="s">
         <v>620</v>
@@ -5382,7 +5382,7 @@
         <v>622</v>
       </c>
       <c r="B31" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C31" t="s">
         <v>1050</v>
@@ -5411,7 +5411,7 @@
         <v>631</v>
       </c>
       <c r="C32" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D32" t="s">
         <v>620</v>
@@ -5440,10 +5440,10 @@
         <v>624</v>
       </c>
       <c r="B33" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C33" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D33" t="s">
         <v>620</v>
@@ -5466,7 +5466,7 @@
         <v>619</v>
       </c>
       <c r="B34" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C34" t="s">
         <v>1045</v>
@@ -5495,10 +5495,10 @@
         <v>628</v>
       </c>
       <c r="B35" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C35" t="s">
         <v>1164</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1165</v>
       </c>
       <c r="D35" t="s">
         <v>620</v>
@@ -5524,7 +5524,7 @@
         <v>630</v>
       </c>
       <c r="B36" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C36" t="s">
         <v>631</v>
@@ -5550,10 +5550,10 @@
         <v>461</v>
       </c>
       <c r="B37" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C37" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>801</v>
@@ -5762,10 +5762,10 @@
         <v>235</v>
       </c>
       <c r="B44" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C44" t="s">
         <v>1092</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1093</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
@@ -5791,10 +5791,10 @@
         <v>238</v>
       </c>
       <c r="B45" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C45" t="s">
         <v>1094</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1095</v>
       </c>
       <c r="D45" t="s">
         <v>71</v>
@@ -5820,10 +5820,10 @@
         <v>290</v>
       </c>
       <c r="B46" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C46" t="s">
         <v>1102</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1103</v>
       </c>
       <c r="D46" t="s">
         <v>71</v>
@@ -5852,10 +5852,10 @@
         <v>319</v>
       </c>
       <c r="B47" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C47" t="s">
         <v>1106</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1107</v>
       </c>
       <c r="D47" t="s">
         <v>71</v>
@@ -5884,10 +5884,10 @@
         <v>616</v>
       </c>
       <c r="B48" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C48" t="s">
         <v>1106</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1107</v>
       </c>
       <c r="D48" t="s">
         <v>71</v>
@@ -5916,10 +5916,10 @@
         <v>683</v>
       </c>
       <c r="B49" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C49" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D49" t="s">
         <v>71</v>
@@ -5951,10 +5951,10 @@
         <v>681</v>
       </c>
       <c r="B50" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C50" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D50" t="s">
         <v>71</v>
@@ -5980,10 +5980,10 @@
         <v>353</v>
       </c>
       <c r="B51" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C51" t="s">
         <v>1112</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1113</v>
       </c>
       <c r="D51" t="s">
         <v>71</v>
@@ -6012,10 +6012,10 @@
         <v>356</v>
       </c>
       <c r="B52" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C52" t="s">
         <v>1114</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1115</v>
       </c>
       <c r="D52" t="s">
         <v>71</v>
@@ -6044,10 +6044,10 @@
         <v>421</v>
       </c>
       <c r="B53" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C53" t="s">
         <v>1122</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1123</v>
       </c>
       <c r="D53" t="s">
         <v>71</v>
@@ -6076,10 +6076,10 @@
         <v>424</v>
       </c>
       <c r="B54" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C54" t="s">
         <v>1124</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1125</v>
       </c>
       <c r="D54" t="s">
         <v>71</v>
@@ -6108,10 +6108,10 @@
         <v>427</v>
       </c>
       <c r="B55" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C55" t="s">
         <v>1126</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1127</v>
       </c>
       <c r="D55" t="s">
         <v>71</v>
@@ -6140,10 +6140,10 @@
         <v>753</v>
       </c>
       <c r="B56" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C56" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D56" t="s">
         <v>71</v>
@@ -6510,10 +6510,10 @@
         <v>316</v>
       </c>
       <c r="B70" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C70" t="s">
         <v>1104</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1105</v>
       </c>
       <c r="D70" t="s">
         <v>317</v>
@@ -6542,7 +6542,7 @@
         <v>1045</v>
       </c>
       <c r="C71" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D71" t="s">
         <v>259</v>
@@ -6603,7 +6603,7 @@
         <v>1045</v>
       </c>
       <c r="C73" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D73" t="s">
         <v>259</v>
@@ -6632,7 +6632,7 @@
         <v>1045</v>
       </c>
       <c r="C74" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D74" t="s">
         <v>259</v>
@@ -6696,7 +6696,7 @@
         <v>1074</v>
       </c>
       <c r="C76" t="s">
-        <v>1075</v>
+        <v>1201</v>
       </c>
       <c r="D76" t="s">
         <v>259</v>
@@ -6722,10 +6722,10 @@
         <v>102</v>
       </c>
       <c r="B77" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C77" t="s">
         <v>1076</v>
-      </c>
-      <c r="C77" t="s">
-        <v>1077</v>
       </c>
       <c r="D77" t="s">
         <v>103</v>
@@ -6748,10 +6748,10 @@
         <v>105</v>
       </c>
       <c r="B78" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C78" t="s">
         <v>1076</v>
-      </c>
-      <c r="C78" t="s">
-        <v>1077</v>
       </c>
       <c r="D78" t="s">
         <v>103</v>
@@ -6774,7 +6774,7 @@
         <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C79" t="s">
         <v>1053</v>
@@ -6800,7 +6800,7 @@
         <v>490</v>
       </c>
       <c r="B80" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C80" t="s">
         <v>440</v>
@@ -6832,7 +6832,7 @@
         <v>492</v>
       </c>
       <c r="B81" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C81" t="s">
         <v>443</v>
@@ -6864,7 +6864,7 @@
         <v>494</v>
       </c>
       <c r="B82" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C82" t="s">
         <v>446</v>
@@ -6896,10 +6896,10 @@
         <v>110</v>
       </c>
       <c r="B83" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C83" t="s">
         <v>1079</v>
-      </c>
-      <c r="C83" t="s">
-        <v>1080</v>
       </c>
       <c r="D83" t="s">
         <v>114</v>
@@ -6925,7 +6925,7 @@
         <v>117</v>
       </c>
       <c r="B84" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C84" t="s">
         <v>1053</v>
@@ -6954,7 +6954,7 @@
         <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C85" t="s">
         <v>1053</v>
@@ -7627,10 +7627,10 @@
         <v>359</v>
       </c>
       <c r="B111" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C111" t="s">
         <v>1116</v>
-      </c>
-      <c r="C111" t="s">
-        <v>1117</v>
       </c>
       <c r="D111" t="s">
         <v>168</v>
@@ -7662,7 +7662,7 @@
         <v>171</v>
       </c>
       <c r="B112" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C112" t="s">
         <v>1053</v>
@@ -7740,10 +7740,10 @@
         <v>241</v>
       </c>
       <c r="B115" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C115" t="s">
         <v>1096</v>
-      </c>
-      <c r="C115" t="s">
-        <v>1097</v>
       </c>
       <c r="D115" t="s">
         <v>176</v>
@@ -7766,7 +7766,7 @@
         <v>175</v>
       </c>
       <c r="B116" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C116" t="s">
         <v>1053</v>
@@ -7792,10 +7792,10 @@
         <v>178</v>
       </c>
       <c r="B117" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C117" t="s">
         <v>1084</v>
-      </c>
-      <c r="C117" t="s">
-        <v>1085</v>
       </c>
       <c r="D117" t="s">
         <v>179</v>
@@ -7818,7 +7818,7 @@
         <v>181</v>
       </c>
       <c r="B118" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C118" t="s">
         <v>1053</v>
@@ -7844,10 +7844,10 @@
         <v>184</v>
       </c>
       <c r="B119" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C119" t="s">
         <v>1087</v>
-      </c>
-      <c r="C119" t="s">
-        <v>1088</v>
       </c>
       <c r="D119" t="s">
         <v>185</v>
@@ -7870,7 +7870,7 @@
         <v>189</v>
       </c>
       <c r="B120" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C120" t="s">
         <v>1053</v>
@@ -8175,10 +8175,10 @@
         <v>480</v>
       </c>
       <c r="B133" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C133" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D133" t="s">
         <v>799</v>
@@ -8204,10 +8204,10 @@
         <v>478</v>
       </c>
       <c r="B134" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C134" t="s">
         <v>1136</v>
-      </c>
-      <c r="C134" t="s">
-        <v>1137</v>
       </c>
       <c r="D134" t="s">
         <v>799</v>
@@ -8233,10 +8233,10 @@
         <v>654</v>
       </c>
       <c r="B135" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C135" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D135" t="s">
         <v>799</v>
@@ -8262,10 +8262,10 @@
         <v>679</v>
       </c>
       <c r="B136" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="C136" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D136" t="s">
         <v>799</v>
@@ -8291,10 +8291,10 @@
         <v>723</v>
       </c>
       <c r="B137" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C137" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D137" t="s">
         <v>799</v>
@@ -8320,7 +8320,7 @@
         <v>534</v>
       </c>
       <c r="B138" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C138" t="s">
         <v>1045</v>
@@ -8352,10 +8352,10 @@
         <v>540</v>
       </c>
       <c r="B139" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C139" t="s">
         <v>1146</v>
-      </c>
-      <c r="C139" t="s">
-        <v>1147</v>
       </c>
       <c r="D139" t="s">
         <v>799</v>
@@ -8384,10 +8384,10 @@
         <v>536</v>
       </c>
       <c r="B140" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C140" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D140" t="s">
         <v>799</v>
@@ -8416,10 +8416,10 @@
         <v>538</v>
       </c>
       <c r="B141" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C141" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D141" t="s">
         <v>799</v>
@@ -8448,7 +8448,7 @@
         <v>193</v>
       </c>
       <c r="C142" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D142" t="s">
         <v>799</v>
@@ -8815,10 +8815,10 @@
         <v>233</v>
       </c>
       <c r="B156" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C156" t="s">
         <v>1090</v>
-      </c>
-      <c r="C156" t="s">
-        <v>1091</v>
       </c>
       <c r="D156" t="s">
         <v>186</v>
@@ -8842,10 +8842,10 @@
         <v>593</v>
       </c>
       <c r="B157" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C157" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D157" t="s">
         <v>236</v>
@@ -8871,7 +8871,7 @@
         <v>589</v>
       </c>
       <c r="B158" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C158" t="s">
         <v>1050</v>
@@ -8897,10 +8897,10 @@
         <v>591</v>
       </c>
       <c r="B159" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C159" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D159" t="s">
         <v>236</v>
@@ -8923,7 +8923,7 @@
         <v>587</v>
       </c>
       <c r="B160" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C160" t="s">
         <v>1045</v>
@@ -8952,10 +8952,10 @@
         <v>595</v>
       </c>
       <c r="B161" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C161" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="D161" t="s">
         <v>236</v>
@@ -8981,10 +8981,10 @@
         <v>603</v>
       </c>
       <c r="B162" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C162" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D162" t="s">
         <v>239</v>
@@ -9010,7 +9010,7 @@
         <v>599</v>
       </c>
       <c r="B163" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C163" t="s">
         <v>1050</v>
@@ -9036,10 +9036,10 @@
         <v>601</v>
       </c>
       <c r="B164" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C164" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D164" t="s">
         <v>239</v>
@@ -9062,7 +9062,7 @@
         <v>597</v>
       </c>
       <c r="B165" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C165" t="s">
         <v>1045</v>
@@ -9091,10 +9091,10 @@
         <v>605</v>
       </c>
       <c r="B166" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C166" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D166" t="s">
         <v>239</v>
@@ -9184,10 +9184,10 @@
         <v>459</v>
       </c>
       <c r="B169" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C169" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D169" t="s">
         <v>16</v>
@@ -9216,7 +9216,7 @@
         <v>453</v>
       </c>
       <c r="B170" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C170" t="s">
         <v>1050</v>
@@ -9245,10 +9245,10 @@
         <v>457</v>
       </c>
       <c r="B171" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C171" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D171" t="s">
         <v>16</v>
@@ -9274,7 +9274,7 @@
         <v>450</v>
       </c>
       <c r="B172" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C172" t="s">
         <v>1045</v>
@@ -9306,10 +9306,10 @@
         <v>455</v>
       </c>
       <c r="B173" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C173" t="s">
         <v>1132</v>
-      </c>
-      <c r="C173" t="s">
-        <v>1133</v>
       </c>
       <c r="D173" t="s">
         <v>16</v>
@@ -9338,10 +9338,10 @@
         <v>472</v>
       </c>
       <c r="B174" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C174" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>16</v>
@@ -9370,7 +9370,7 @@
         <v>466</v>
       </c>
       <c r="B175" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C175" t="s">
         <v>1050</v>
@@ -9399,10 +9399,10 @@
         <v>468</v>
       </c>
       <c r="B176" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C176" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>16</v>
@@ -9428,7 +9428,7 @@
         <v>463</v>
       </c>
       <c r="B177" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C177" t="s">
         <v>1045</v>
@@ -9460,10 +9460,10 @@
         <v>476</v>
       </c>
       <c r="B178" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C178" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>16</v>
@@ -9489,10 +9489,10 @@
         <v>470</v>
       </c>
       <c r="B179" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C179" t="s">
         <v>1135</v>
-      </c>
-      <c r="C179" t="s">
-        <v>1136</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>16</v>
@@ -9518,10 +9518,10 @@
         <v>474</v>
       </c>
       <c r="B180" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C180" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>16</v>
@@ -9547,7 +9547,7 @@
         <v>635</v>
       </c>
       <c r="B181" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C181" t="s">
         <v>443</v>
@@ -9579,10 +9579,10 @@
         <v>505</v>
       </c>
       <c r="B182" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C182" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D182" t="s">
         <v>16</v>
@@ -9611,7 +9611,7 @@
         <v>499</v>
       </c>
       <c r="B183" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C183" t="s">
         <v>1050</v>
@@ -9640,10 +9640,10 @@
         <v>501</v>
       </c>
       <c r="B184" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C184" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D184" t="s">
         <v>16</v>
@@ -9669,7 +9669,7 @@
         <v>496</v>
       </c>
       <c r="B185" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C185" t="s">
         <v>1045</v>
@@ -9701,10 +9701,10 @@
         <v>503</v>
       </c>
       <c r="B186" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C186" t="s">
         <v>1143</v>
-      </c>
-      <c r="C186" t="s">
-        <v>1144</v>
       </c>
       <c r="D186" t="s">
         <v>16</v>
@@ -9733,7 +9733,7 @@
         <v>485</v>
       </c>
       <c r="B187" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C187" t="s">
         <v>244</v>
@@ -9762,10 +9762,10 @@
         <v>544</v>
       </c>
       <c r="B188" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C188" t="s">
         <v>1151</v>
-      </c>
-      <c r="C188" t="s">
-        <v>1152</v>
       </c>
       <c r="D188" t="s">
         <v>16</v>
@@ -9794,10 +9794,10 @@
         <v>574</v>
       </c>
       <c r="B189" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C189" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D189" t="s">
         <v>16</v>
@@ -9826,7 +9826,7 @@
         <v>570</v>
       </c>
       <c r="B190" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C190" t="s">
         <v>1050</v>
@@ -9855,10 +9855,10 @@
         <v>572</v>
       </c>
       <c r="B191" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C191" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D191" t="s">
         <v>16</v>
@@ -9884,7 +9884,7 @@
         <v>567</v>
       </c>
       <c r="B192" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C192" t="s">
         <v>1045</v>
@@ -9916,10 +9916,10 @@
         <v>576</v>
       </c>
       <c r="B193" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C193" t="s">
         <v>1156</v>
-      </c>
-      <c r="C193" t="s">
-        <v>1157</v>
       </c>
       <c r="D193" t="s">
         <v>16</v>
@@ -9948,7 +9948,7 @@
         <v>578</v>
       </c>
       <c r="B194" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C194" t="s">
         <v>1045</v>
@@ -9980,10 +9980,10 @@
         <v>581</v>
       </c>
       <c r="B195" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C195" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D195" t="s">
         <v>16</v>
@@ -10009,10 +10009,10 @@
         <v>733</v>
       </c>
       <c r="B196" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C196" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D196" t="s">
         <v>16</v>
@@ -10041,7 +10041,7 @@
         <v>729</v>
       </c>
       <c r="B197" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C197" t="s">
         <v>1050</v>
@@ -10070,10 +10070,10 @@
         <v>731</v>
       </c>
       <c r="B198" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C198" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D198" t="s">
         <v>16</v>
@@ -10099,7 +10099,7 @@
         <v>727</v>
       </c>
       <c r="B199" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C199" t="s">
         <v>1045</v>
@@ -10131,10 +10131,10 @@
         <v>735</v>
       </c>
       <c r="B200" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C200" t="s">
         <v>1185</v>
-      </c>
-      <c r="C200" t="s">
-        <v>1186</v>
       </c>
       <c r="D200" t="s">
         <v>16</v>
@@ -10160,7 +10160,7 @@
         <v>609</v>
       </c>
       <c r="B201" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C201" t="s">
         <v>440</v>
@@ -10192,7 +10192,7 @@
         <v>612</v>
       </c>
       <c r="B202" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C202" t="s">
         <v>443</v>
@@ -10224,7 +10224,7 @@
         <v>614</v>
       </c>
       <c r="B203" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C203" t="s">
         <v>446</v>
@@ -10256,10 +10256,10 @@
         <v>488</v>
       </c>
       <c r="B204" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C204" t="s">
         <v>1141</v>
-      </c>
-      <c r="C204" t="s">
-        <v>1142</v>
       </c>
       <c r="D204" t="s">
         <v>16</v>
@@ -10285,10 +10285,10 @@
         <v>638</v>
       </c>
       <c r="B205" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C205" t="s">
         <v>1167</v>
-      </c>
-      <c r="C205" t="s">
-        <v>1168</v>
       </c>
       <c r="D205" t="s">
         <v>16</v>
@@ -10317,10 +10317,10 @@
         <v>772</v>
       </c>
       <c r="B206" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C206" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>16</v>
@@ -10355,7 +10355,7 @@
         <v>352</v>
       </c>
       <c r="C207" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D207" t="s">
         <v>16</v>
@@ -10381,10 +10381,10 @@
         <v>648</v>
       </c>
       <c r="B208" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C208" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D208" t="s">
         <v>16</v>
@@ -10413,7 +10413,7 @@
         <v>644</v>
       </c>
       <c r="B209" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C209" t="s">
         <v>1050</v>
@@ -10442,10 +10442,10 @@
         <v>646</v>
       </c>
       <c r="B210" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C210" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D210" t="s">
         <v>16</v>
@@ -10471,7 +10471,7 @@
         <v>641</v>
       </c>
       <c r="B211" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C211" t="s">
         <v>1045</v>
@@ -10503,10 +10503,10 @@
         <v>652</v>
       </c>
       <c r="B212" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C212" t="s">
         <v>1169</v>
-      </c>
-      <c r="C212" t="s">
-        <v>1170</v>
       </c>
       <c r="D212" t="s">
         <v>16</v>
@@ -10535,10 +10535,10 @@
         <v>650</v>
       </c>
       <c r="B213" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C213" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D213" t="s">
         <v>16</v>
@@ -10564,10 +10564,10 @@
         <v>673</v>
       </c>
       <c r="B214" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C214" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D214" t="s">
         <v>16</v>
@@ -10596,7 +10596,7 @@
         <v>669</v>
       </c>
       <c r="B215" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C215" t="s">
         <v>1050</v>
@@ -10625,10 +10625,10 @@
         <v>671</v>
       </c>
       <c r="B216" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C216" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D216" t="s">
         <v>16</v>
@@ -10654,7 +10654,7 @@
         <v>666</v>
       </c>
       <c r="B217" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C217" t="s">
         <v>1045</v>
@@ -10686,10 +10686,10 @@
         <v>677</v>
       </c>
       <c r="B218" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C218" t="s">
         <v>1173</v>
-      </c>
-      <c r="C218" t="s">
-        <v>1174</v>
       </c>
       <c r="D218" t="s">
         <v>16</v>
@@ -10718,10 +10718,10 @@
         <v>675</v>
       </c>
       <c r="B219" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C219" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D219" t="s">
         <v>16</v>
@@ -10747,10 +10747,10 @@
         <v>585</v>
       </c>
       <c r="B220" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C220" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>16</v>
@@ -10782,10 +10782,10 @@
         <v>583</v>
       </c>
       <c r="B221" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C221" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>16</v>
@@ -10814,10 +10814,10 @@
         <v>662</v>
       </c>
       <c r="B222" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C222" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D222" t="s">
         <v>16</v>
@@ -10846,7 +10846,7 @@
         <v>658</v>
       </c>
       <c r="B223" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C223" t="s">
         <v>1050</v>
@@ -10875,10 +10875,10 @@
         <v>660</v>
       </c>
       <c r="B224" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C224" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D224" t="s">
         <v>16</v>
@@ -10904,7 +10904,7 @@
         <v>656</v>
       </c>
       <c r="B225" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C225" t="s">
         <v>1045</v>
@@ -10936,10 +10936,10 @@
         <v>664</v>
       </c>
       <c r="B226" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C226" t="s">
         <v>1171</v>
-      </c>
-      <c r="C226" t="s">
-        <v>1172</v>
       </c>
       <c r="D226" t="s">
         <v>16</v>
@@ -10968,10 +10968,10 @@
         <v>685</v>
       </c>
       <c r="B227" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C227" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D227" t="s">
         <v>16</v>
@@ -11000,10 +11000,10 @@
         <v>717</v>
       </c>
       <c r="B228" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C228" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D228" t="s">
         <v>16</v>
@@ -11032,7 +11032,7 @@
         <v>713</v>
       </c>
       <c r="B229" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C229" t="s">
         <v>1050</v>
@@ -11061,10 +11061,10 @@
         <v>715</v>
       </c>
       <c r="B230" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C230" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D230" t="s">
         <v>16</v>
@@ -11090,7 +11090,7 @@
         <v>710</v>
       </c>
       <c r="B231" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C231" t="s">
         <v>1045</v>
@@ -11122,10 +11122,10 @@
         <v>721</v>
       </c>
       <c r="B232" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C232" t="s">
         <v>1181</v>
-      </c>
-      <c r="C232" t="s">
-        <v>1182</v>
       </c>
       <c r="D232" t="s">
         <v>16</v>
@@ -11154,10 +11154,10 @@
         <v>719</v>
       </c>
       <c r="B233" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C233" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D233" t="s">
         <v>16</v>
@@ -11183,10 +11183,10 @@
         <v>516</v>
       </c>
       <c r="B234" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C234" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D234" t="s">
         <v>16</v>
@@ -11215,7 +11215,7 @@
         <v>510</v>
       </c>
       <c r="B235" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C235" t="s">
         <v>1050</v>
@@ -11244,10 +11244,10 @@
         <v>512</v>
       </c>
       <c r="B236" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C236" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D236" t="s">
         <v>16</v>
@@ -11273,7 +11273,7 @@
         <v>507</v>
       </c>
       <c r="B237" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C237" t="s">
         <v>1045</v>
@@ -11305,10 +11305,10 @@
         <v>520</v>
       </c>
       <c r="B238" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C238" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D238" t="s">
         <v>16</v>
@@ -11337,10 +11337,10 @@
         <v>514</v>
       </c>
       <c r="B239" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C239" t="s">
         <v>1145</v>
-      </c>
-      <c r="C239" t="s">
-        <v>1146</v>
       </c>
       <c r="D239" t="s">
         <v>16</v>
@@ -11369,10 +11369,10 @@
         <v>518</v>
       </c>
       <c r="B240" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C240" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D240" t="s">
         <v>16</v>
@@ -11398,10 +11398,10 @@
         <v>528</v>
       </c>
       <c r="B241" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C241" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D241" t="s">
         <v>16</v>
@@ -11430,7 +11430,7 @@
         <v>524</v>
       </c>
       <c r="B242" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C242" t="s">
         <v>1050</v>
@@ -11459,10 +11459,10 @@
         <v>526</v>
       </c>
       <c r="B243" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C243" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D243" t="s">
         <v>16</v>
@@ -11488,7 +11488,7 @@
         <v>522</v>
       </c>
       <c r="B244" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C244" t="s">
         <v>1045</v>
@@ -11520,10 +11520,10 @@
         <v>532</v>
       </c>
       <c r="B245" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C245" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D245" t="s">
         <v>16</v>
@@ -11552,10 +11552,10 @@
         <v>530</v>
       </c>
       <c r="B246" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C246" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D246" t="s">
         <v>16</v>
@@ -11581,7 +11581,7 @@
         <v>737</v>
       </c>
       <c r="B247" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C247" t="s">
         <v>440</v>
@@ -11613,7 +11613,7 @@
         <v>740</v>
       </c>
       <c r="B248" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C248" t="s">
         <v>443</v>
@@ -11645,7 +11645,7 @@
         <v>742</v>
       </c>
       <c r="B249" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C249" t="s">
         <v>446</v>
@@ -11677,10 +11677,10 @@
         <v>756</v>
       </c>
       <c r="B250" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C250" t="s">
         <v>1191</v>
-      </c>
-      <c r="C250" t="s">
-        <v>1192</v>
       </c>
       <c r="D250" t="s">
         <v>16</v>
@@ -11709,10 +11709,10 @@
         <v>482</v>
       </c>
       <c r="B251" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C251" t="s">
         <v>1138</v>
-      </c>
-      <c r="C251" t="s">
-        <v>1139</v>
       </c>
       <c r="D251" t="s">
         <v>16</v>
@@ -11741,10 +11741,10 @@
         <v>765</v>
       </c>
       <c r="B252" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C252" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D252" t="s">
         <v>16</v>
@@ -11773,7 +11773,7 @@
         <v>761</v>
       </c>
       <c r="B253" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C253" t="s">
         <v>1050</v>
@@ -11802,10 +11802,10 @@
         <v>763</v>
       </c>
       <c r="B254" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C254" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D254" t="s">
         <v>16</v>
@@ -11831,7 +11831,7 @@
         <v>758</v>
       </c>
       <c r="B255" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C255" t="s">
         <v>1045</v>
@@ -11863,10 +11863,10 @@
         <v>767</v>
       </c>
       <c r="B256" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C256" t="s">
         <v>1193</v>
-      </c>
-      <c r="C256" t="s">
-        <v>1194</v>
       </c>
       <c r="D256" t="s">
         <v>16</v>
@@ -11895,10 +11895,10 @@
         <v>769</v>
       </c>
       <c r="B257" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C257" t="s">
         <v>1195</v>
-      </c>
-      <c r="C257" t="s">
-        <v>1196</v>
       </c>
       <c r="D257" t="s">
         <v>16</v>
@@ -11927,10 +11927,10 @@
         <v>781</v>
       </c>
       <c r="B258" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C258" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D258" t="s">
         <v>16</v>
@@ -11959,7 +11959,7 @@
         <v>777</v>
       </c>
       <c r="B259" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C259" t="s">
         <v>1050</v>
@@ -11988,10 +11988,10 @@
         <v>779</v>
       </c>
       <c r="B260" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C260" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D260" t="s">
         <v>16</v>
@@ -12017,7 +12017,7 @@
         <v>774</v>
       </c>
       <c r="B261" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C261" t="s">
         <v>1045</v>
@@ -12049,10 +12049,10 @@
         <v>783</v>
       </c>
       <c r="B262" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C262" t="s">
         <v>1198</v>
-      </c>
-      <c r="C262" t="s">
-        <v>1199</v>
       </c>
       <c r="D262" t="s">
         <v>16</v>
@@ -12081,7 +12081,7 @@
         <v>1053</v>
       </c>
       <c r="C263" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D263" t="s">
         <v>16</v>
@@ -12156,7 +12156,7 @@
         <v>1053</v>
       </c>
       <c r="C266" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D266" t="s">
         <v>16</v>
@@ -12286,7 +12286,7 @@
         <v>16</v>
       </c>
       <c r="C271" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D271" t="s">
         <v>16</v>
@@ -12341,7 +12341,7 @@
         <v>1053</v>
       </c>
       <c r="C273" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D273" t="s">
         <v>16</v>
@@ -12390,10 +12390,10 @@
         <v>607</v>
       </c>
       <c r="B275" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C275" t="s">
         <v>1161</v>
-      </c>
-      <c r="C275" t="s">
-        <v>1162</v>
       </c>
       <c r="D275" t="s">
         <v>16</v>
@@ -12448,7 +12448,7 @@
         <v>1053</v>
       </c>
       <c r="C277" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D277" t="s">
         <v>16</v>
@@ -12529,7 +12529,7 @@
         <v>16</v>
       </c>
       <c r="C280" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D280" t="s">
         <v>16</v>
@@ -12613,7 +12613,7 @@
         <v>1053</v>
       </c>
       <c r="C283" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D283" t="s">
         <v>16</v>
@@ -12977,10 +12977,10 @@
         <v>693</v>
       </c>
       <c r="B297" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C297" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>803</v>
@@ -13006,7 +13006,7 @@
         <v>689</v>
       </c>
       <c r="B298" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C298" t="s">
         <v>1050</v>
@@ -13032,10 +13032,10 @@
         <v>691</v>
       </c>
       <c r="B299" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C299" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>803</v>
@@ -13058,7 +13058,7 @@
         <v>687</v>
       </c>
       <c r="B300" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C300" t="s">
         <v>1045</v>
@@ -13087,10 +13087,10 @@
         <v>695</v>
       </c>
       <c r="B301" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C301" t="s">
         <v>1176</v>
-      </c>
-      <c r="C301" t="s">
-        <v>1177</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>803</v>
@@ -13428,10 +13428,10 @@
         <v>345</v>
       </c>
       <c r="B314" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C314" t="s">
         <v>1108</v>
-      </c>
-      <c r="C314" t="s">
-        <v>1109</v>
       </c>
       <c r="D314" t="s">
         <v>346</v>
@@ -13457,10 +13457,10 @@
         <v>704</v>
       </c>
       <c r="B315" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C315" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D315" t="s">
         <v>698</v>
@@ -13486,7 +13486,7 @@
         <v>700</v>
       </c>
       <c r="B316" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C316" t="s">
         <v>1050</v>
@@ -13512,10 +13512,10 @@
         <v>702</v>
       </c>
       <c r="B317" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C317" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D317" t="s">
         <v>698</v>
@@ -13538,7 +13538,7 @@
         <v>697</v>
       </c>
       <c r="B318" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C318" t="s">
         <v>1045</v>
@@ -13567,10 +13567,10 @@
         <v>706</v>
       </c>
       <c r="B319" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C319" t="s">
         <v>1178</v>
-      </c>
-      <c r="C319" t="s">
-        <v>1179</v>
       </c>
       <c r="D319" t="s">
         <v>698</v>
@@ -13596,10 +13596,10 @@
         <v>708</v>
       </c>
       <c r="B320" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C320" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="D320" t="s">
         <v>698</v>
@@ -13622,7 +13622,7 @@
         <v>362</v>
       </c>
       <c r="B321" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C321" t="s">
         <v>1053</v>
@@ -13807,10 +13807,10 @@
         <v>725</v>
       </c>
       <c r="B328" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C328" t="s">
         <v>1183</v>
-      </c>
-      <c r="C328" t="s">
-        <v>1184</v>
       </c>
       <c r="D328" t="s">
         <v>55</v>
@@ -14304,7 +14304,7 @@
         <v>420</v>
       </c>
       <c r="B347" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C347" t="s">
         <v>16</v>
@@ -14333,10 +14333,10 @@
         <v>448</v>
       </c>
       <c r="B348" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C348" t="s">
         <v>1130</v>
-      </c>
-      <c r="C348" t="s">
-        <v>1131</v>
       </c>
       <c r="D348" t="s">
         <v>288</v>
@@ -14394,7 +14394,7 @@
         <v>288</v>
       </c>
       <c r="C350" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D350" t="s">
         <v>288</v>
@@ -14423,7 +14423,7 @@
         <v>288</v>
       </c>
       <c r="C351" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D351" t="s">
         <v>288</v>
@@ -14452,7 +14452,7 @@
         <v>193</v>
       </c>
       <c r="C352" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D352" s="1" t="s">
         <v>193</v>
@@ -14468,6 +14468,9 @@
       </c>
       <c r="I352" t="s">
         <v>752</v>
+      </c>
+      <c r="K352" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L352" t="s">
         <v>1038</v>
@@ -14495,6 +14498,9 @@
       <c r="I353" t="s">
         <v>748</v>
       </c>
+      <c r="K353" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="L353" t="s">
         <v>1038</v>
       </c>
@@ -14507,7 +14513,7 @@
         <v>193</v>
       </c>
       <c r="C354" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D354" s="1" t="s">
         <v>193</v>
@@ -14520,6 +14526,9 @@
       </c>
       <c r="I354" t="s">
         <v>750</v>
+      </c>
+      <c r="K354" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L354" t="s">
         <v>1038</v>

</xml_diff>

<commit_message>
reverse json generation and menus working
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DD3CEB-9A6C-E043-B449-0AF7FD06F81C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F483E735-B84E-4542-A3D6-AB32F4D72180}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38360" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3106" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="1202">
   <si>
     <t>Amharic-Latin-BGN.xml</t>
   </si>
@@ -4510,8 +4510,8 @@
   <dimension ref="A1:M355"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D352" sqref="A352:XFD354"/>
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9744,7 +9744,10 @@
       <c r="E187" t="s">
         <v>486</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F187" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G187" t="s">
         <v>244</v>
       </c>
       <c r="H187" t="s">
@@ -12113,6 +12116,9 @@
         <v>16</v>
       </c>
       <c r="F264" t="s">
+        <v>16</v>
+      </c>
+      <c r="G264" t="s">
         <v>244</v>
       </c>
       <c r="H264" t="s">

</xml_diff>

<commit_message>
"Validate" action added. "Close" and "Close All" introduced.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F483E735-B84E-4542-A3D6-AB32F4D72180}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C0C00-0339-4D41-B310-3834CE2DD764}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38360" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3109" uniqueCount="1203">
   <si>
     <t>Amharic-Latin-BGN.xml</t>
   </si>
@@ -3626,6 +3626,9 @@
   </si>
   <si>
     <t>Aethiopica_Latn</t>
+  </si>
+  <si>
+    <t>Han-Spacedhan</t>
   </si>
 </sst>
 </file>
@@ -4509,9 +4512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L112" sqref="L112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7679,6 +7682,9 @@
       <c r="I112" t="s">
         <v>172</v>
       </c>
+      <c r="L112" t="s">
+        <v>1202</v>
+      </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">

</xml_diff>

<commit_message>
Start of gemination work.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40FF369-6A07-7142-A98A-12E30A259A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F0F345-3C86-1C4F-9B07-30AE415F815B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="11480" windowWidth="38360" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="9860" windowWidth="38360" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICU Transliterations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3198" uniqueCount="1253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="1255">
   <si>
     <t>Amharic-Latin-BGN.xml</t>
   </si>
@@ -3730,9 +3730,6 @@
     <t>Latin-Ethiopic/ALA</t>
   </si>
   <si>
-    <t>Latin-Ethiopic/BetaMetsehaf</t>
-  </si>
-  <si>
     <t>Latin-Ethiopic/ES3842</t>
   </si>
   <si>
@@ -3760,9 +3757,6 @@
     <t>TekieAlibekit_Ethi</t>
   </si>
   <si>
-    <t>Latin-Ethiopic/TekieAlibekit</t>
-  </si>
-  <si>
     <t>Ethiopic-Latin-TekieAlibekit.xml</t>
   </si>
   <si>
@@ -3779,6 +3773,18 @@
   </si>
   <si>
     <t>Musnad</t>
+  </si>
+  <si>
+    <t>Blin</t>
+  </si>
+  <si>
+    <t>Tigrinya.ER</t>
+  </si>
+  <si>
+    <t>Latin-Ethiopic/Tekie_Alibekit</t>
+  </si>
+  <si>
+    <t>Latin-Ethiopic/Beta_Metsehaf</t>
   </si>
 </sst>
 </file>
@@ -4671,7 +4677,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
+      <selection pane="bottomLeft" activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6932,7 +6938,7 @@
         <v>1224</v>
       </c>
       <c r="J78" t="s">
-        <v>1236</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
@@ -6943,7 +6949,7 @@
         <v>1073</v>
       </c>
       <c r="C79" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="D79" t="s">
         <v>259</v>
@@ -6958,10 +6964,10 @@
         <v>6</v>
       </c>
       <c r="I79" t="s">
+        <v>1240</v>
+      </c>
+      <c r="J79" t="s">
         <v>1241</v>
-      </c>
-      <c r="J79" t="s">
-        <v>1242</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -6984,13 +6990,13 @@
         <v>1218</v>
       </c>
       <c r="H80" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I80" t="s">
         <v>1223</v>
       </c>
       <c r="J80" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
@@ -7019,7 +7025,7 @@
         <v>1222</v>
       </c>
       <c r="J81" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
@@ -7035,6 +7041,9 @@
       <c r="D82" t="s">
         <v>259</v>
       </c>
+      <c r="E82" t="s">
+        <v>1251</v>
+      </c>
       <c r="F82" t="s">
         <v>16</v>
       </c>
@@ -7053,31 +7062,34 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="B83" t="s">
         <v>1073</v>
       </c>
       <c r="C83" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D83" t="s">
         <v>259</v>
       </c>
+      <c r="E83" t="s">
+        <v>1251</v>
+      </c>
       <c r="F83" t="s">
         <v>16</v>
       </c>
       <c r="G83" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="H83" t="s">
         <v>6</v>
       </c>
       <c r="I83" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>1246</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -7088,10 +7100,13 @@
         <v>1073</v>
       </c>
       <c r="C84" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="D84" t="s">
         <v>259</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1252</v>
       </c>
       <c r="F84" t="s">
         <v>71</v>
@@ -7140,28 +7155,28 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B86" t="s">
         <v>1073</v>
       </c>
       <c r="C86" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="D86" t="s">
         <v>259</v>
       </c>
       <c r="F86" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="H86" t="s">
         <v>6</v>
       </c>
       <c r="I86" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="J86" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updates to process ethiopic gemination mark.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F0F345-3C86-1C4F-9B07-30AE415F815B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17DF87B-5D70-6F4C-A82C-1FE2645C4F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="9860" windowWidth="38360" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38360" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICU Transliterations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="1255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="1255">
   <si>
     <t>Amharic-Latin-BGN.xml</t>
   </si>
@@ -3667,9 +3667,6 @@
     <t>Ethiopic-Latin/ALA</t>
   </si>
   <si>
-    <t>Ethiopic-Latin-Braille.xml</t>
-  </si>
-  <si>
     <t>BetaMetsehaf</t>
   </si>
   <si>
@@ -3785,6 +3782,9 @@
   </si>
   <si>
     <t>Latin-Ethiopic/Beta_Metsehaf</t>
+  </si>
+  <si>
+    <t>Ethiopic-Braille-Amharic.xml</t>
   </si>
 </sst>
 </file>
@@ -4675,9 +4675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6880,7 +6880,7 @@
         <v>1042</v>
       </c>
       <c r="J76" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
@@ -6891,7 +6891,7 @@
         <v>1073</v>
       </c>
       <c r="C77" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="D77" t="s">
         <v>259</v>
@@ -6909,7 +6909,7 @@
         <v>1214</v>
       </c>
       <c r="J77" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
@@ -6920,7 +6920,7 @@
         <v>1073</v>
       </c>
       <c r="C78" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D78" t="s">
         <v>259</v>
@@ -6929,33 +6929,36 @@
         <v>16</v>
       </c>
       <c r="G78" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="H78" t="s">
         <v>6</v>
       </c>
       <c r="I78" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J78" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>1215</v>
+        <v>1254</v>
       </c>
       <c r="B79" t="s">
         <v>1073</v>
       </c>
       <c r="C79" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="D79" t="s">
         <v>259</v>
       </c>
+      <c r="E79" t="s">
+        <v>1</v>
+      </c>
       <c r="F79" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="G79" t="s">
         <v>1</v>
@@ -6964,10 +6967,10 @@
         <v>6</v>
       </c>
       <c r="I79" t="s">
+        <v>1239</v>
+      </c>
+      <c r="J79" t="s">
         <v>1240</v>
-      </c>
-      <c r="J79" t="s">
-        <v>1241</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -6978,7 +6981,7 @@
         <v>1073</v>
       </c>
       <c r="C80" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="D80" t="s">
         <v>259</v>
@@ -6987,16 +6990,16 @@
         <v>16</v>
       </c>
       <c r="G80" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H80" t="s">
         <v>3</v>
       </c>
       <c r="I80" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="J80" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
@@ -7007,7 +7010,7 @@
         <v>1073</v>
       </c>
       <c r="C81" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D81" t="s">
         <v>259</v>
@@ -7016,16 +7019,16 @@
         <v>16</v>
       </c>
       <c r="G81" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="H81" t="s">
         <v>6</v>
       </c>
       <c r="I81" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J81" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
@@ -7036,60 +7039,60 @@
         <v>1073</v>
       </c>
       <c r="C82" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="D82" t="s">
         <v>259</v>
       </c>
       <c r="E82" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
       </c>
       <c r="G82" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="H82" t="s">
         <v>6</v>
       </c>
       <c r="I82" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="J82" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B83" t="s">
         <v>1073</v>
       </c>
       <c r="C83" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="D83" t="s">
         <v>259</v>
       </c>
       <c r="E83" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
       </c>
       <c r="G83" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="H83" t="s">
         <v>6</v>
       </c>
       <c r="I83" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -7100,13 +7103,13 @@
         <v>1073</v>
       </c>
       <c r="C84" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="D84" t="s">
         <v>259</v>
       </c>
       <c r="E84" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="F84" t="s">
         <v>71</v>
@@ -7121,7 +7124,7 @@
         <v>1212</v>
       </c>
       <c r="J84" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
@@ -7132,7 +7135,7 @@
         <v>1073</v>
       </c>
       <c r="C85" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="D85" t="s">
         <v>259</v>
@@ -7150,33 +7153,33 @@
         <v>1211</v>
       </c>
       <c r="J85" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B86" t="s">
         <v>1073</v>
       </c>
       <c r="C86" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="D86" t="s">
         <v>259</v>
       </c>
       <c r="F86" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="H86" t="s">
         <v>6</v>
       </c>
       <c r="I86" t="s">
+        <v>1247</v>
+      </c>
+      <c r="J86" t="s">
         <v>1248</v>
-      </c>
-      <c r="J86" t="s">
-        <v>1249</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update for Braille menu change under Amharic only.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17DF87B-5D70-6F4C-A82C-1FE2645C4F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D57E79-F687-2E4F-981D-0EA9560184CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38360" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="1255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="1255">
   <si>
     <t>Amharic-Latin-BGN.xml</t>
   </si>
@@ -4677,7 +4677,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6960,9 +6960,6 @@
       <c r="F79" t="s">
         <v>1216</v>
       </c>
-      <c r="G79" t="s">
-        <v>1</v>
-      </c>
       <c r="H79" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Resync with latest CLDR. Support for U+135D and U+135E.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ICU-Transliterations.xlsx
+++ b/src/main/resources/data/ICU-Transliterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/Xliterator/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D57E79-F687-2E4F-981D-0EA9560184CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63C6B10-93B2-9F4A-967E-5671FF8C23E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38360" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="5920" windowWidth="38360" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICU Transliterations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="1255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="1258">
   <si>
     <t>Amharic-Latin-BGN.xml</t>
   </si>
@@ -3785,13 +3785,22 @@
   </si>
   <si>
     <t>Ethiopic-Braille-Amharic.xml</t>
+  </si>
+  <si>
+    <t>Myanmar-Latin.xml</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Myanmar-Latin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3946,6 +3955,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -4310,7 +4325,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -4318,6 +4333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4673,11 +4689,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M365"/>
+  <dimension ref="A1:M366"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
+      <pane ySplit="1" topLeftCell="A295" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D307" sqref="D307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13443,44 +13459,41 @@
         <v>907</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>693</v>
+        <v>1255</v>
       </c>
       <c r="B307" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
       <c r="C307" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D307" s="2" t="s">
-        <v>803</v>
+        <v>1052</v>
+      </c>
+      <c r="D307" t="s">
+        <v>620</v>
+      </c>
+      <c r="E307" t="s">
+        <v>1256</v>
       </c>
       <c r="F307" t="s">
-        <v>13</v>
-      </c>
-      <c r="G307" t="s">
-        <v>349</v>
+        <v>16</v>
       </c>
       <c r="H307" t="s">
         <v>3</v>
       </c>
-      <c r="I307" t="s">
-        <v>694</v>
-      </c>
-      <c r="L307" t="s">
-        <v>1015</v>
+      <c r="I307" s="7" t="s">
+        <v>1257</v>
       </c>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="B308" t="s">
         <v>1173</v>
       </c>
       <c r="C308" t="s">
-        <v>1049</v>
+        <v>1108</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>803</v>
@@ -13488,479 +13501,479 @@
       <c r="F308" t="s">
         <v>13</v>
       </c>
+      <c r="G308" t="s">
+        <v>349</v>
+      </c>
       <c r="H308" t="s">
         <v>3</v>
       </c>
       <c r="I308" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="L308" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B309" t="s">
         <v>1173</v>
       </c>
       <c r="C309" t="s">
-        <v>1127</v>
+        <v>1049</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>803</v>
       </c>
       <c r="F309" t="s">
-        <v>801</v>
+        <v>13</v>
       </c>
       <c r="H309" t="s">
         <v>3</v>
       </c>
       <c r="I309" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="L309" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="B310" t="s">
         <v>1173</v>
       </c>
       <c r="C310" t="s">
-        <v>1044</v>
+        <v>1127</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>803</v>
       </c>
       <c r="F310" t="s">
-        <v>259</v>
-      </c>
-      <c r="G310" t="s">
-        <v>1</v>
+        <v>801</v>
       </c>
       <c r="H310" t="s">
         <v>3</v>
       </c>
       <c r="I310" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="L310" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="B311" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="C311" t="s">
-        <v>1175</v>
+        <v>1044</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>803</v>
       </c>
       <c r="F311" t="s">
-        <v>799</v>
-      </c>
-      <c r="G311" s="2" t="s">
-        <v>803</v>
+        <v>259</v>
+      </c>
+      <c r="G311" t="s">
+        <v>1</v>
       </c>
       <c r="H311" t="s">
         <v>3</v>
       </c>
       <c r="I311" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="L311" t="s">
-        <v>1038</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>322</v>
+        <v>695</v>
       </c>
       <c r="B312" t="s">
-        <v>1065</v>
+        <v>1174</v>
       </c>
       <c r="C312" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D312" t="s">
-        <v>52</v>
+        <v>1175</v>
+      </c>
+      <c r="D312" s="2" t="s">
+        <v>803</v>
       </c>
       <c r="F312" t="s">
-        <v>13</v>
+        <v>799</v>
+      </c>
+      <c r="G312" s="2" t="s">
+        <v>803</v>
       </c>
       <c r="H312" t="s">
         <v>3</v>
       </c>
       <c r="I312" t="s">
-        <v>323</v>
+        <v>696</v>
       </c>
       <c r="L312" t="s">
-        <v>908</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B313" t="s">
         <v>1065</v>
       </c>
       <c r="C313" t="s">
-        <v>1059</v>
+        <v>1051</v>
       </c>
       <c r="D313" t="s">
         <v>52</v>
       </c>
       <c r="F313" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H313" t="s">
         <v>3</v>
       </c>
       <c r="I313" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L313" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B314" t="s">
         <v>1065</v>
       </c>
       <c r="C314" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D314" t="s">
         <v>52</v>
       </c>
       <c r="F314" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H314" t="s">
         <v>3</v>
       </c>
       <c r="I314" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L314" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="315" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B315" t="s">
         <v>1065</v>
       </c>
       <c r="C315" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D315" t="s">
         <v>52</v>
       </c>
       <c r="F315" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H315" t="s">
         <v>3</v>
       </c>
       <c r="I315" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L315" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B316" t="s">
         <v>1065</v>
       </c>
       <c r="C316" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D316" t="s">
         <v>52</v>
       </c>
       <c r="F316" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H316" t="s">
         <v>3</v>
       </c>
       <c r="I316" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L316" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B317" t="s">
-        <v>52</v>
+        <v>1065</v>
       </c>
       <c r="C317" t="s">
-        <v>41</v>
+        <v>1062</v>
       </c>
       <c r="D317" t="s">
         <v>52</v>
       </c>
       <c r="F317" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H317" t="s">
         <v>3</v>
       </c>
-      <c r="K317" t="s">
-        <v>42</v>
+      <c r="I317" t="s">
+        <v>331</v>
       </c>
       <c r="L317" t="s">
-        <v>1038</v>
+        <v>912</v>
       </c>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B318" t="s">
-        <v>1065</v>
+        <v>52</v>
       </c>
       <c r="C318" t="s">
-        <v>1063</v>
+        <v>41</v>
       </c>
       <c r="D318" t="s">
         <v>52</v>
       </c>
       <c r="F318" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H318" t="s">
         <v>3</v>
       </c>
-      <c r="I318" t="s">
-        <v>334</v>
+      <c r="K318" t="s">
+        <v>42</v>
       </c>
       <c r="L318" t="s">
-        <v>913</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B319" t="s">
         <v>1065</v>
       </c>
       <c r="C319" t="s">
-        <v>1052</v>
+        <v>1063</v>
       </c>
       <c r="D319" t="s">
         <v>52</v>
       </c>
       <c r="F319" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="H319" t="s">
         <v>3</v>
       </c>
       <c r="I319" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="L319" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B320" t="s">
         <v>1065</v>
       </c>
       <c r="C320" t="s">
-        <v>1064</v>
+        <v>1052</v>
       </c>
       <c r="D320" t="s">
         <v>52</v>
       </c>
       <c r="F320" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H320" t="s">
         <v>3</v>
       </c>
       <c r="I320" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="L320" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B321" t="s">
         <v>1065</v>
       </c>
       <c r="C321" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="D321" t="s">
         <v>52</v>
       </c>
       <c r="F321" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H321" t="s">
         <v>3</v>
       </c>
       <c r="I321" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L321" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B322" t="s">
         <v>1065</v>
       </c>
       <c r="C322" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D322" t="s">
         <v>52</v>
       </c>
       <c r="F322" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H322" t="s">
         <v>3</v>
       </c>
       <c r="I322" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="L322" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B323" t="s">
         <v>1065</v>
       </c>
       <c r="C323" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D323" t="s">
         <v>52</v>
       </c>
       <c r="F323" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H323" t="s">
         <v>3</v>
       </c>
       <c r="I323" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="L323" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B324" t="s">
-        <v>1106</v>
+        <v>1065</v>
       </c>
       <c r="C324" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="D324" t="s">
-        <v>346</v>
+        <v>52</v>
       </c>
       <c r="F324" t="s">
-        <v>16</v>
-      </c>
-      <c r="G324" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H324" t="s">
         <v>3</v>
       </c>
       <c r="I324" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="L324" t="s">
-        <v>1038</v>
+        <v>918</v>
       </c>
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>704</v>
+        <v>345</v>
       </c>
       <c r="B325" t="s">
-        <v>1176</v>
+        <v>1106</v>
       </c>
       <c r="C325" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D325" t="s">
-        <v>698</v>
+        <v>346</v>
       </c>
       <c r="F325" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G325" t="s">
-        <v>349</v>
+        <v>2</v>
       </c>
       <c r="H325" t="s">
         <v>3</v>
       </c>
       <c r="I325" t="s">
-        <v>705</v>
+        <v>347</v>
       </c>
       <c r="L325" t="s">
-        <v>1019</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="B326" t="s">
         <v>1176</v>
       </c>
       <c r="C326" t="s">
-        <v>1049</v>
+        <v>1108</v>
       </c>
       <c r="D326" t="s">
         <v>698</v>
@@ -13968,121 +13981,124 @@
       <c r="F326" t="s">
         <v>13</v>
       </c>
+      <c r="G326" t="s">
+        <v>349</v>
+      </c>
       <c r="H326" t="s">
         <v>3</v>
       </c>
       <c r="I326" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="L326" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B327" t="s">
         <v>1176</v>
       </c>
       <c r="C327" t="s">
-        <v>1127</v>
+        <v>1049</v>
       </c>
       <c r="D327" t="s">
         <v>698</v>
       </c>
       <c r="F327" t="s">
-        <v>801</v>
+        <v>13</v>
       </c>
       <c r="H327" t="s">
         <v>3</v>
       </c>
       <c r="I327" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="L327" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="B328" t="s">
         <v>1176</v>
       </c>
       <c r="C328" t="s">
-        <v>1044</v>
+        <v>1127</v>
       </c>
       <c r="D328" t="s">
         <v>698</v>
       </c>
       <c r="F328" t="s">
-        <v>259</v>
-      </c>
-      <c r="G328" t="s">
-        <v>1</v>
+        <v>801</v>
       </c>
       <c r="H328" t="s">
         <v>3</v>
       </c>
       <c r="I328" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="L328" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
       <c r="B329" t="s">
         <v>1176</v>
       </c>
       <c r="C329" t="s">
-        <v>1177</v>
+        <v>1044</v>
       </c>
       <c r="D329" t="s">
         <v>698</v>
       </c>
       <c r="F329" t="s">
-        <v>799</v>
+        <v>259</v>
       </c>
       <c r="G329" t="s">
-        <v>698</v>
+        <v>1</v>
       </c>
       <c r="H329" t="s">
         <v>3</v>
       </c>
       <c r="I329" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="L329" t="s">
-        <v>1038</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B330" t="s">
         <v>1176</v>
       </c>
       <c r="C330" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D330" t="s">
         <v>698</v>
       </c>
       <c r="F330" t="s">
-        <v>16</v>
+        <v>799</v>
+      </c>
+      <c r="G330" t="s">
+        <v>698</v>
       </c>
       <c r="H330" t="s">
         <v>3</v>
       </c>
       <c r="I330" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="L330" t="s">
         <v>1038</v>
@@ -14090,28 +14106,25 @@
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>362</v>
+        <v>708</v>
       </c>
       <c r="B331" t="s">
-        <v>1116</v>
+        <v>1176</v>
       </c>
       <c r="C331" t="s">
-        <v>1052</v>
+        <v>1178</v>
       </c>
       <c r="D331" t="s">
-        <v>363</v>
+        <v>698</v>
       </c>
       <c r="F331" t="s">
         <v>16</v>
       </c>
       <c r="H331" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I331" t="s">
-        <v>364</v>
-      </c>
-      <c r="J331" t="s">
-        <v>365</v>
+        <v>709</v>
       </c>
       <c r="L331" t="s">
         <v>1038</v>
@@ -14119,184 +14132,184 @@
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B332" t="s">
-        <v>1066</v>
+        <v>1116</v>
       </c>
       <c r="C332" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D332" t="s">
-        <v>55</v>
+        <v>363</v>
       </c>
       <c r="F332" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H332" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I332" t="s">
-        <v>367</v>
+        <v>364</v>
+      </c>
+      <c r="J332" t="s">
+        <v>365</v>
       </c>
       <c r="L332" t="s">
-        <v>919</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B333" t="s">
         <v>1066</v>
       </c>
       <c r="C333" t="s">
-        <v>1059</v>
+        <v>1051</v>
       </c>
       <c r="D333" t="s">
         <v>55</v>
       </c>
       <c r="F333" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H333" t="s">
         <v>3</v>
       </c>
       <c r="I333" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L333" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B334" t="s">
         <v>1066</v>
       </c>
       <c r="C334" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D334" t="s">
         <v>55</v>
       </c>
       <c r="F334" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H334" t="s">
         <v>3</v>
       </c>
       <c r="I334" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L334" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B335" t="s">
         <v>1066</v>
       </c>
       <c r="C335" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D335" t="s">
         <v>55</v>
       </c>
       <c r="F335" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H335" t="s">
         <v>3</v>
       </c>
       <c r="I335" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L335" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B336" t="s">
         <v>1066</v>
       </c>
       <c r="C336" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D336" t="s">
         <v>55</v>
       </c>
       <c r="F336" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H336" t="s">
         <v>3</v>
       </c>
       <c r="I336" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L336" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="337" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B337" t="s">
-        <v>55</v>
+        <v>1066</v>
       </c>
       <c r="C337" t="s">
-        <v>41</v>
+        <v>1062</v>
       </c>
       <c r="D337" t="s">
         <v>55</v>
       </c>
       <c r="F337" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H337" t="s">
         <v>3</v>
       </c>
-      <c r="K337" t="s">
-        <v>42</v>
+      <c r="I337" t="s">
+        <v>375</v>
       </c>
       <c r="L337" t="s">
-        <v>1038</v>
+        <v>923</v>
       </c>
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>725</v>
+        <v>376</v>
       </c>
       <c r="B338" t="s">
-        <v>1181</v>
+        <v>55</v>
       </c>
       <c r="C338" t="s">
-        <v>1182</v>
+        <v>41</v>
       </c>
       <c r="D338" t="s">
         <v>55</v>
       </c>
       <c r="F338" t="s">
-        <v>799</v>
-      </c>
-      <c r="G338" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="H338" t="s">
         <v>3</v>
       </c>
-      <c r="I338" t="s">
-        <v>726</v>
+      <c r="K338" t="s">
+        <v>42</v>
       </c>
       <c r="L338" t="s">
         <v>1038</v>
@@ -14304,528 +14317,525 @@
     </row>
     <row r="339" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>377</v>
+        <v>725</v>
       </c>
       <c r="B339" t="s">
-        <v>1066</v>
+        <v>1181</v>
       </c>
       <c r="C339" t="s">
-        <v>1063</v>
+        <v>1182</v>
       </c>
       <c r="D339" t="s">
         <v>55</v>
       </c>
       <c r="F339" t="s">
-        <v>44</v>
+        <v>799</v>
+      </c>
+      <c r="G339" t="s">
+        <v>55</v>
       </c>
       <c r="H339" t="s">
         <v>3</v>
       </c>
       <c r="I339" t="s">
-        <v>378</v>
+        <v>726</v>
       </c>
       <c r="L339" t="s">
-        <v>924</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="340" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B340" t="s">
         <v>1066</v>
       </c>
       <c r="C340" t="s">
-        <v>1052</v>
+        <v>1063</v>
       </c>
       <c r="D340" t="s">
         <v>55</v>
       </c>
       <c r="F340" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="H340" t="s">
         <v>3</v>
       </c>
       <c r="I340" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L340" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="341" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B341" t="s">
         <v>1066</v>
       </c>
       <c r="C341" t="s">
-        <v>1064</v>
+        <v>1052</v>
       </c>
       <c r="D341" t="s">
         <v>55</v>
       </c>
       <c r="F341" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H341" t="s">
         <v>3</v>
       </c>
       <c r="I341" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L341" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B342" t="s">
         <v>1066</v>
       </c>
       <c r="C342" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D342" t="s">
         <v>55</v>
       </c>
       <c r="F342" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H342" t="s">
         <v>3</v>
       </c>
       <c r="I342" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L342" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="343" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B343" t="s">
         <v>1066</v>
       </c>
       <c r="C343" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D343" t="s">
         <v>55</v>
       </c>
       <c r="F343" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H343" t="s">
         <v>3</v>
       </c>
       <c r="I343" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L343" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="344" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B344" t="s">
         <v>1066</v>
       </c>
       <c r="C344" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D344" t="s">
         <v>55</v>
       </c>
       <c r="F344" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H344" t="s">
         <v>3</v>
       </c>
       <c r="I344" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L344" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="345" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B345" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C345" t="s">
-        <v>1051</v>
+        <v>1068</v>
       </c>
       <c r="D345" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F345" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="H345" t="s">
         <v>3</v>
       </c>
       <c r="I345" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L345" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="346" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B346" t="s">
         <v>1067</v>
       </c>
       <c r="C346" t="s">
-        <v>1059</v>
+        <v>1051</v>
       </c>
       <c r="D346" t="s">
         <v>58</v>
       </c>
       <c r="F346" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H346" t="s">
         <v>3</v>
       </c>
       <c r="I346" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L346" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="347" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B347" t="s">
         <v>1067</v>
       </c>
       <c r="C347" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D347" t="s">
         <v>58</v>
       </c>
       <c r="F347" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H347" t="s">
         <v>3</v>
       </c>
       <c r="I347" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L347" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B348" t="s">
         <v>1067</v>
       </c>
       <c r="C348" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D348" t="s">
         <v>58</v>
       </c>
       <c r="F348" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H348" t="s">
         <v>3</v>
       </c>
       <c r="I348" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L348" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="349" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B349" t="s">
         <v>1067</v>
       </c>
       <c r="C349" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D349" t="s">
         <v>58</v>
       </c>
       <c r="F349" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H349" t="s">
         <v>3</v>
       </c>
       <c r="I349" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L349" t="s">
-        <v>1038</v>
+        <v>933</v>
       </c>
     </row>
     <row r="350" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B350" t="s">
-        <v>58</v>
+        <v>1067</v>
       </c>
       <c r="C350" t="s">
-        <v>41</v>
+        <v>1062</v>
       </c>
       <c r="D350" t="s">
         <v>58</v>
       </c>
       <c r="F350" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H350" t="s">
         <v>3</v>
       </c>
-      <c r="K350" t="s">
-        <v>42</v>
+      <c r="I350" t="s">
+        <v>398</v>
       </c>
       <c r="L350" t="s">
-        <v>934</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="351" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B351" t="s">
-        <v>1067</v>
+        <v>58</v>
       </c>
       <c r="C351" t="s">
-        <v>1063</v>
+        <v>41</v>
       </c>
       <c r="D351" t="s">
         <v>58</v>
       </c>
       <c r="F351" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H351" t="s">
         <v>3</v>
       </c>
-      <c r="I351" t="s">
-        <v>401</v>
+      <c r="K351" t="s">
+        <v>42</v>
       </c>
       <c r="L351" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="352" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B352" t="s">
         <v>1067</v>
       </c>
       <c r="C352" t="s">
-        <v>1052</v>
+        <v>1063</v>
       </c>
       <c r="D352" t="s">
         <v>58</v>
       </c>
       <c r="F352" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="H352" t="s">
         <v>3</v>
       </c>
       <c r="I352" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="L352" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B353" t="s">
         <v>1067</v>
       </c>
       <c r="C353" t="s">
-        <v>1064</v>
+        <v>1052</v>
       </c>
       <c r="D353" t="s">
         <v>58</v>
       </c>
       <c r="F353" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H353" t="s">
         <v>3</v>
       </c>
       <c r="I353" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L353" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B354" t="s">
         <v>1067</v>
       </c>
       <c r="C354" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D354" t="s">
         <v>58</v>
       </c>
       <c r="F354" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H354" t="s">
         <v>3</v>
       </c>
       <c r="I354" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="L354" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="355" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B355" t="s">
         <v>1067</v>
       </c>
       <c r="C355" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D355" t="s">
         <v>58</v>
       </c>
       <c r="F355" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H355" t="s">
         <v>3</v>
       </c>
       <c r="I355" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L355" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B356" t="s">
         <v>1067</v>
       </c>
       <c r="C356" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="D356" t="s">
         <v>58</v>
       </c>
       <c r="F356" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H356" t="s">
         <v>3</v>
       </c>
       <c r="I356" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="L356" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="B357" t="s">
-        <v>1118</v>
+        <v>1067</v>
       </c>
       <c r="C357" t="s">
-        <v>16</v>
+        <v>1068</v>
       </c>
       <c r="D357" t="s">
-        <v>288</v>
-      </c>
-      <c r="E357" t="s">
-        <v>798</v>
+        <v>58</v>
       </c>
       <c r="F357" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="H357" t="s">
-        <v>6</v>
-      </c>
-      <c r="K357" t="s">
-        <v>42</v>
+        <v>3</v>
+      </c>
+      <c r="I357" t="s">
+        <v>411</v>
       </c>
       <c r="L357" t="s">
-        <v>1038</v>
+        <v>940</v>
       </c>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>448</v>
+        <v>420</v>
       </c>
       <c r="B358" t="s">
-        <v>1128</v>
+        <v>1118</v>
       </c>
       <c r="C358" t="s">
-        <v>1129</v>
+        <v>16</v>
       </c>
       <c r="D358" t="s">
         <v>288</v>
       </c>
-      <c r="E358" s="2" t="s">
-        <v>807</v>
+      <c r="E358" t="s">
+        <v>798</v>
       </c>
       <c r="F358" t="s">
-        <v>799</v>
-      </c>
-      <c r="G358" s="2" t="s">
-        <v>807</v>
+        <v>16</v>
       </c>
       <c r="H358" t="s">
-        <v>3</v>
-      </c>
-      <c r="I358" t="s">
-        <v>449</v>
+        <v>6</v>
+      </c>
+      <c r="K358" t="s">
+        <v>42</v>
       </c>
       <c r="L358" t="s">
         <v>1038</v>
@@ -14833,68 +14843,71 @@
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>416</v>
+        <v>448</v>
       </c>
       <c r="B359" t="s">
-        <v>288</v>
+        <v>1128</v>
       </c>
       <c r="C359" t="s">
-        <v>1052</v>
+        <v>1129</v>
       </c>
       <c r="D359" t="s">
         <v>288</v>
       </c>
+      <c r="E359" s="2" t="s">
+        <v>807</v>
+      </c>
       <c r="F359" t="s">
-        <v>16</v>
+        <v>799</v>
+      </c>
+      <c r="G359" s="2" t="s">
+        <v>807</v>
       </c>
       <c r="H359" t="s">
         <v>3</v>
       </c>
       <c r="I359" t="s">
-        <v>417</v>
+        <v>449</v>
       </c>
       <c r="L359" t="s">
-        <v>941</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B360" t="s">
         <v>288</v>
       </c>
       <c r="C360" t="s">
-        <v>1118</v>
+        <v>1052</v>
       </c>
       <c r="D360" t="s">
         <v>288</v>
       </c>
       <c r="F360" t="s">
-        <v>288</v>
-      </c>
-      <c r="G360" t="s">
-        <v>798</v>
+        <v>16</v>
       </c>
       <c r="H360" t="s">
-        <v>6</v>
-      </c>
-      <c r="K360" t="s">
-        <v>42</v>
+        <v>3</v>
+      </c>
+      <c r="I360" t="s">
+        <v>417</v>
       </c>
       <c r="L360" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B361" t="s">
         <v>288</v>
       </c>
       <c r="C361" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D361" t="s">
         <v>288</v>
@@ -14903,7 +14916,7 @@
         <v>288</v>
       </c>
       <c r="G361" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H361" t="s">
         <v>6</v>
@@ -14912,35 +14925,32 @@
         <v>42</v>
       </c>
       <c r="L361" t="s">
-        <v>1038</v>
+        <v>942</v>
       </c>
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>751</v>
+        <v>419</v>
       </c>
       <c r="B362" t="s">
-        <v>193</v>
+        <v>288</v>
       </c>
       <c r="C362" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D362" s="1" t="s">
-        <v>193</v>
+        <v>1119</v>
+      </c>
+      <c r="D362" t="s">
+        <v>288</v>
       </c>
       <c r="F362" t="s">
-        <v>13</v>
+        <v>288</v>
       </c>
       <c r="G362" t="s">
-        <v>349</v>
+        <v>800</v>
       </c>
       <c r="H362" t="s">
-        <v>3</v>
-      </c>
-      <c r="I362" t="s">
-        <v>752</v>
-      </c>
-      <c r="K362" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K362" t="s">
         <v>42</v>
       </c>
       <c r="L362" t="s">
@@ -14949,13 +14959,13 @@
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B363" t="s">
         <v>193</v>
       </c>
       <c r="C363" t="s">
-        <v>1049</v>
+        <v>1108</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>193</v>
@@ -14963,11 +14973,14 @@
       <c r="F363" t="s">
         <v>13</v>
       </c>
+      <c r="G363" t="s">
+        <v>349</v>
+      </c>
       <c r="H363" t="s">
         <v>3</v>
       </c>
       <c r="I363" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="K363" s="1" t="s">
         <v>42</v>
@@ -14978,25 +14991,25 @@
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B364" t="s">
         <v>193</v>
       </c>
       <c r="C364" t="s">
-        <v>1127</v>
+        <v>1049</v>
       </c>
       <c r="D364" s="1" t="s">
         <v>193</v>
       </c>
       <c r="F364" t="s">
-        <v>801</v>
+        <v>13</v>
       </c>
       <c r="H364" t="s">
         <v>3</v>
       </c>
       <c r="I364" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="K364" s="1" t="s">
         <v>42</v>
@@ -15007,36 +15020,65 @@
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
+        <v>749</v>
+      </c>
+      <c r="B365" t="s">
+        <v>193</v>
+      </c>
+      <c r="C365" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F365" t="s">
+        <v>801</v>
+      </c>
+      <c r="H365" t="s">
+        <v>3</v>
+      </c>
+      <c r="I365" t="s">
+        <v>750</v>
+      </c>
+      <c r="K365" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L365" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="366" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A366" t="s">
         <v>66</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B366" t="s">
         <v>1052</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C366" t="s">
         <v>1071</v>
       </c>
-      <c r="D365" t="s">
+      <c r="D366" t="s">
         <v>67</v>
       </c>
-      <c r="F365" t="s">
-        <v>16</v>
-      </c>
-      <c r="H365" t="s">
+      <c r="F366" t="s">
+        <v>16</v>
+      </c>
+      <c r="H366" t="s">
         <v>6</v>
       </c>
-      <c r="I365" t="s">
+      <c r="I366" t="s">
         <v>68</v>
       </c>
-      <c r="J365" t="s">
+      <c r="J366" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M370">
-    <sortCondition ref="D2:D370"/>
-    <sortCondition ref="E2:E370"/>
-    <sortCondition ref="F2:F370"/>
-    <sortCondition ref="G2:G370"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M371">
+    <sortCondition ref="D2:D371"/>
+    <sortCondition ref="E2:E371"/>
+    <sortCondition ref="F2:F371"/>
+    <sortCondition ref="G2:G371"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>